<commit_message>
named ranges and countingiter implemented
</commit_message>
<xml_diff>
--- a/scripts/data/Job Ship Dates.xlsx
+++ b/scripts/data/Job Ship Dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PMiller1\git\prodctrlcore\scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{5B231AC8-C03D-4D4D-98F0-A10DC7189AAD}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{AE24B4F2-0F63-4142-BE3C-6D509F772235}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="3435" yWindow="3045" windowWidth="21600" windowHeight="11385" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-120" yWindow="-120" windowWidth="29040" windowHeight="15840" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dates" sheetId="1" r:id="rId1"/>
@@ -18,6 +18,12 @@
     <sheet name="Products" sheetId="3" r:id="rId3"/>
     <sheet name="Bays" sheetId="6" r:id="rId4"/>
   </sheets>
+  <definedNames>
+    <definedName name="BAYS_HEADER">Bays!$A$1:$C$1</definedName>
+    <definedName name="DATES_HEADER">Dates!$A$1:$C$1</definedName>
+    <definedName name="PM_HEADER">PM!$A$1:$B$1</definedName>
+    <definedName name="PRODUCTS_HEADER">Products!$A$1:$C$1</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <pivotCaches>
     <pivotCache cacheId="6" r:id="rId5"/>
@@ -775,26 +781,35 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43983.633046643517" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43984.290078356484" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="3">
+  <cacheFields count="2">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
-      <sharedItems count="199">
+      <sharedItems count="200">
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160230F-06]" c="D-1160230F-06"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160245A-02]" c="D-1160245A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160245A-13]" c="D-1160245A-13"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-01]" c="D-1160253A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-02]" c="D-1160253A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-04]" c="D-1160253C-04"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-05]" c="D-1160253C-05"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-06]" c="D-1160253C-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-07]" c="D-1160253C-07"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032A-01]" c="D-1170032A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032A-02]" c="D-1170032A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032B-03]" c="D-1170032B-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170082A-03]" c="D-1170082A-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170082D-08]" c="D-1170082D-08"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-02]" c="D-1170143C-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-03]" c="D-1170143C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-04]" c="D-1170143C-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155A-01]" c="D-1170155A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155D-04]" c="D-1170155D-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155G-13]" c="D-1170155G-13"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217A-01]" c="D-1170217A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217C-03]" c="D-1170217C-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217F-07]" c="D-1170217F-07"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217G-08]" c="D-1170217G-08"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272A-01]" c="D-1170272A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272B-02]" c="D-1170272B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272C-03]" c="D-1170272C-03"/>
@@ -815,11 +830,13 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180081A-02]" c="D-1180081A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180091C-03]" c="D-1180091C-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180091C-04]" c="D-1180091C-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095C-03]" c="D-1180095C-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095D-04]" c="D-1180095D-04"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095D-05]" c="D-1180095D-05"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095E-06]" c="D-1180095E-06"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095G-08]" c="D-1180095G-08"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095H-09]" c="D-1180095H-09"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095J-10]" c="D-1180095J-10"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095L-12]" c="D-1180095L-12"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180116B-01]" c="D-1180116B-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180136A-01]" c="D-1180136A-01"/>
@@ -841,12 +858,19 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201F-09]" c="D-1180201F-09"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201G-10]" c="D-1180201G-10"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201H-11]" c="D-1180201H-11"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238A-01]" c="D-1180238A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238B-02]" c="D-1180238B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238C-03]" c="D-1180238C-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238D-04]" c="D-1180238D-04"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238D-05]" c="D-1180238D-05"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238E-06]" c="D-1180238E-06"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238E-07]" c="D-1180238E-07"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238F-08]" c="D-1180238F-08"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238G-09]" c="D-1180238G-09"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180246A-01]" c="D-1180246A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-01]" c="D-1180261A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-02]" c="D-1180261A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180262A-02]" c="D-1180262A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180274A-02]" c="D-1180274A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285A-01]" c="D-1180285A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285C-03]" c="D-1180285C-03"/>
@@ -861,6 +885,7 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190028A-01]" c="D-1190028A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190028B-02]" c="D-1190028B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190036A-01]" c="D-1190036A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190037A-01]" c="D-1190037A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190038A-01]" c="D-1190038A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190060A-01]" c="D-1190060A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190066A-01]" c="D-1190066A-01"/>
@@ -889,9 +914,11 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190138A-01]" c="D-1190138A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190144A-01]" c="D-1190144A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190144B-02]" c="D-1190144B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190145A-01]" c="D-1190145A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190148A-01]" c="D-1190148A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190165A-01]" c="D-1190165A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190179A-01]" c="D-1190179A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190187A-01]" c="D-1190187A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190193A-01]" c="D-1190193A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190196A-01]" c="D-1190196A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190203A-01]" c="D-1190203A-01"/>
@@ -927,6 +954,680 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190272A-01]" c="D-1190272A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190272B-02]" c="D-1190272B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274A-01]" c="D-1190274A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274B-02]" c="D-1190274B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278A-01]" c="D-1190278A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278B-02]" c="D-1190278B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278C-03]" c="D-1190278C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278C-04]" c="D-1190278C-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278C-05]" c="D-1190278C-05"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278D-06]" c="D-1190278D-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278D-07]" c="D-1190278D-07"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278E-08]" c="D-1190278E-08"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278E-09]" c="D-1190278E-09"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278F-10]" c="D-1190278F-10"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278G-11]" c="D-1190278G-11"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190279A-01]" c="D-1190279A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190283A-01]" c="D-1190283A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190289A-01]" c="D-1190289A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190295A-01]" c="D-1190295A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190300A-01]" c="D-1190300A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190305A-01]" c="D-1190305A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190306A-01]" c="D-1190306A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190310A-01]" c="D-1190310A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190310B-02]" c="D-1190310B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190320A-01]" c="D-1190320A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190321A-01]" c="D-1190321A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200014A-01]" c="D-1200014A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200017A-01]" c="D-1200017A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200017A-02]" c="D-1200017A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200021A-01]" c="D-1200021A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200022A-01]" c="D-1200022A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200023A-01]" c="D-1200023A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200031A-01]" c="D-1200031A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200034A-01]" c="D-1200034A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200089A-03]" c="D-1200089A-03"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Job Shipments].[PM Initials].[PM Initials]" caption="PM Initials" numFmtId="0" hierarchy="50" level="1">
+      <sharedItems count="7">
+        <s v="[Job Shipments].[PM Initials].&amp;[MK]" c="MK"/>
+        <s v="[Job Shipments].[PM Initials].&amp;[DP]" c="DP"/>
+        <s v="[Job Shipments].[PM Initials].&amp;[JF]" c="JF"/>
+        <s v="[Job Shipments].[PM Initials].&amp;[JW]" c="JW"/>
+        <s v="[Job Shipments].[PM Initials].&amp;[KG]" c="KG"/>
+        <s v="[Job Shipments].[PM Initials].&amp;[MD]" c="MD"/>
+        <s v="[Job Shipments].[PM Initials].&amp;" c=""/>
+      </sharedItems>
+    </cacheField>
+  </cacheFields>
+  <cacheHierarchies count="390">
+    <cacheHierarchy uniqueName="[Calendar].[Calendar Date]" caption="Calendar Date" attribute="1" defaultMemberUniqueName="[Calendar].[Calendar Date].[All]" allUniqueName="[Calendar].[Calendar Date].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Month Ending]" caption="Month Ending" attribute="1" defaultMemberUniqueName="[Calendar].[Month Ending].[All]" allUniqueName="[Calendar].[Month Ending].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Month Name]" caption="Month Name" attribute="1" defaultMemberUniqueName="[Calendar].[Month Name].[All]" allUniqueName="[Calendar].[Month Name].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Month Number]" caption="Month Number" attribute="1" defaultMemberUniqueName="[Calendar].[Month Number].[All]" allUniqueName="[Calendar].[Month Number].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Month Short Name]" caption="Month Short Name" attribute="1" defaultMemberUniqueName="[Calendar].[Month Short Name].[All]" allUniqueName="[Calendar].[Month Short Name].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Month Starting]" caption="Month Starting" attribute="1" defaultMemberUniqueName="[Calendar].[Month Starting].[All]" allUniqueName="[Calendar].[Month Starting].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Month Year]" caption="Month Year" attribute="1" defaultMemberUniqueName="[Calendar].[Month Year].[All]" allUniqueName="[Calendar].[Month Year].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Months Out]" caption="Months Out" attribute="1" defaultMemberUniqueName="[Calendar].[Months Out].[All]" allUniqueName="[Calendar].[Months Out].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Calendar].[Quarter].[All]" allUniqueName="[Calendar].[Quarter].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Week Beginning]" caption="Week Beginning" attribute="1" defaultMemberUniqueName="[Calendar].[Week Beginning].[All]" allUniqueName="[Calendar].[Week Beginning].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Week Ending]" caption="Week Ending" attribute="1" defaultMemberUniqueName="[Calendar].[Week Ending].[All]" allUniqueName="[Calendar].[Week Ending].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Weeks Out]" caption="Weeks Out" attribute="1" defaultMemberUniqueName="[Calendar].[Weeks Out].[All]" allUniqueName="[Calendar].[Weeks Out].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Calendar].[Year].[All]" allUniqueName="[Calendar].[Year].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Year Month]" caption="Year Month" attribute="1" defaultMemberUniqueName="[Calendar].[Year Month].[All]" allUniqueName="[Calendar].[Year Month].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Calendar].[Year Qtr]" caption="Year Qtr" attribute="1" defaultMemberUniqueName="[Calendar].[Year Qtr].[All]" allUniqueName="[Calendar].[Year Qtr].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[Bay]" caption="Bay" attribute="1" defaultMemberUniqueName="[Cost Centers].[Bay].[All]" allUniqueName="[Cost Centers].[Bay].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[Cost Center]" caption="Cost Center" attribute="1" defaultMemberUniqueName="[Cost Centers].[Cost Center].[All]" allUniqueName="[Cost Centers].[Cost Center].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[Cost Center Display]" caption="Cost Center Display" attribute="1" defaultMemberUniqueName="[Cost Centers].[Cost Center Display].[All]" allUniqueName="[Cost Centers].[Cost Center Display].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[Cost Center Name]" caption="Cost Center Name" attribute="1" defaultMemberUniqueName="[Cost Centers].[Cost Center Name].[All]" allUniqueName="[Cost Centers].[Cost Center Name].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[Facility]" caption="Facility" attribute="1" defaultMemberUniqueName="[Cost Centers].[Facility].[All]" allUniqueName="[Cost Centers].[Facility].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[Plant]" caption="Plant" attribute="1" defaultMemberUniqueName="[Cost Centers].[Plant].[All]" allUniqueName="[Cost Centers].[Plant].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[Work Center]" caption="Work Center" attribute="1" defaultMemberUniqueName="[Cost Centers].[Work Center].[All]" allUniqueName="[Cost Centers].[Work Center].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[Work Center Display]" caption="Work Center Display" attribute="1" defaultMemberUniqueName="[Cost Centers].[Work Center Display].[All]" allUniqueName="[Cost Centers].[Work Center Display].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[Work Center Name]" caption="Work Center Name" attribute="1" defaultMemberUniqueName="[Cost Centers].[Work Center Name].[All]" allUniqueName="[Cost Centers].[Work Center Name].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Functions].[Function Code]" caption="Function Code" attribute="1" defaultMemberUniqueName="[Functions].[Function Code].[All]" allUniqueName="[Functions].[Function Code].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Functions].[Function Description]" caption="Function Description" attribute="1" defaultMemberUniqueName="[Functions].[Function Description].[All]" allUniqueName="[Functions].[Function Description].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Functions].[Function Display]" caption="Function Display" attribute="1" defaultMemberUniqueName="[Functions].[Function Display].[All]" allUniqueName="[Functions].[Function Display].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Functions].[Function Group]" caption="Function Group" attribute="1" defaultMemberUniqueName="[Functions].[Function Group].[All]" allUniqueName="[Functions].[Function Group].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[Finish Date Mismatch]" caption="Finish Date Mismatch" attribute="1" defaultMemberUniqueName="[HD Schedule].[Finish Date Mismatch].[All]" allUniqueName="[HD Schedule].[Finish Date Mismatch].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[Start Date Mismatch]" caption="Start Date Mismatch" attribute="1" defaultMemberUniqueName="[HD Schedule].[Start Date Mismatch].[All]" allUniqueName="[HD Schedule].[Start Date Mismatch].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[Task Code]" caption="Task Code" attribute="1" defaultMemberUniqueName="[HD Schedule].[Task Code].[All]" allUniqueName="[HD Schedule].[Task Code].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[Task Name]" caption="Task Name" attribute="1" defaultMemberUniqueName="[HD Schedule].[Task Name].[All]" allUniqueName="[HD Schedule].[Task Name].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[Task Name Short]" caption="Task Name Short" attribute="1" defaultMemberUniqueName="[HD Schedule].[Task Name Short].[All]" allUniqueName="[HD Schedule].[Task Name Short].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[Task Start Date]" caption="Task Start Date" attribute="1" defaultMemberUniqueName="[HD Schedule].[Task Start Date].[All]" allUniqueName="[HD Schedule].[Task Start Date].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Coating]" caption="Coating" attribute="1" defaultMemberUniqueName="[Job Shipments].[Coating].[All]" allUniqueName="[Job Shipments].[Coating].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Coating Desc]" caption="Coating Desc" attribute="1" defaultMemberUniqueName="[Job Shipments].[Coating Desc].[All]" allUniqueName="[Job Shipments].[Coating Desc].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Display Ship Date]" caption="Display Ship Date" attribute="1" defaultMemberUniqueName="[Job Shipments].[Display Ship Date].[All]" allUniqueName="[Job Shipments].[Display Ship Date].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[First Start Date]" caption="First Start Date" attribute="1" defaultMemberUniqueName="[Job Shipments].[First Start Date].[All]" allUniqueName="[Job Shipments].[First Start Date].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[HD Ship Date]" caption="HD Ship Date" attribute="1" defaultMemberUniqueName="[Job Shipments].[HD Ship Date].[All]" allUniqueName="[Job Shipments].[HD Ship Date].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[In HD?]" caption="In HD?" attribute="1" defaultMemberUniqueName="[Job Shipments].[In HD?].[All]" allUniqueName="[Job Shipments].[In HD?].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Job Name]" caption="Job Name" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Name].[All]" allUniqueName="[Job Shipments].[Job Name].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Job Number]" caption="Job Number" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Number].[All]" allUniqueName="[Job Shipments].[Job Number].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Job State]" caption="Job State" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job State].[All]" allUniqueName="[Job Shipments].[Job State].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Job Status]" caption="Job Status" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Status].[All]" allUniqueName="[Job Shipments].[Job Status].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Job Status Full Text]" caption="Job Status Full Text" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Status Full Text].[All]" allUniqueName="[Job Shipments].[Job Status Full Text].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Job Structure Shipment]" caption="Job Structure Shipment" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Structure Shipment].[All]" allUniqueName="[Job Shipments].[Job Structure Shipment].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="0"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Job Shipments].[Milestone Status Text]" caption="Milestone Status Text" attribute="1" defaultMemberUniqueName="[Job Shipments].[Milestone Status Text].[All]" allUniqueName="[Job Shipments].[Milestone Status Text].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[P6 Ship Date]" caption="P6 Ship Date" attribute="1" defaultMemberUniqueName="[Job Shipments].[P6 Ship Date].[All]" allUniqueName="[Job Shipments].[P6 Ship Date].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[P6 Ship Month Year]" caption="P6 Ship Month Year" attribute="1" defaultMemberUniqueName="[Job Shipments].[P6 Ship Month Year].[All]" allUniqueName="[Job Shipments].[P6 Ship Month Year].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[P6 Ship Year Month]" caption="P6 Ship Year Month" attribute="1" defaultMemberUniqueName="[Job Shipments].[P6 Ship Year Month].[All]" allUniqueName="[Job Shipments].[P6 Ship Year Month].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[PM Initials]" caption="PM Initials" attribute="1" defaultMemberUniqueName="[Job Shipments].[PM Initials].[All]" allUniqueName="[Job Shipments].[PM Initials].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="2" unbalanced="0">
+      <fieldsUsage count="2">
+        <fieldUsage x="-1"/>
+        <fieldUsage x="1"/>
+      </fieldsUsage>
+    </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Job Shipments].[Production Status]" caption="Production Status" attribute="1" defaultMemberUniqueName="[Job Shipments].[Production Status].[All]" allUniqueName="[Job Shipments].[Production Status].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Project Manager]" caption="Project Manager" attribute="1" defaultMemberUniqueName="[Job Shipments].[Project Manager].[All]" allUniqueName="[Job Shipments].[Project Manager].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Project Milestone Status]" caption="Project Milestone Status" attribute="1" defaultMemberUniqueName="[Job Shipments].[Project Milestone Status].[All]" allUniqueName="[Job Shipments].[Project Milestone Status].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Project Notes]" caption="Project Notes" attribute="1" defaultMemberUniqueName="[Job Shipments].[Project Notes].[All]" allUniqueName="[Job Shipments].[Project Notes].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Project Ship Date Status]" caption="Project Ship Date Status" attribute="1" defaultMemberUniqueName="[Job Shipments].[Project Ship Date Status].[All]" allUniqueName="[Job Shipments].[Project Ship Date Status].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Ship Date Job Label]" caption="Ship Date Job Label" attribute="1" defaultMemberUniqueName="[Job Shipments].[Ship Date Job Label].[All]" allUniqueName="[Job Shipments].[Ship Date Job Label].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Ship Date Status Text]" caption="Ship Date Status Text" attribute="1" defaultMemberUniqueName="[Job Shipments].[Ship Date Status Text].[All]" allUniqueName="[Job Shipments].[Ship Date Status Text].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Ship Dates Match?]" caption="Ship Dates Match?" attribute="1" defaultMemberUniqueName="[Job Shipments].[Ship Dates Match?].[All]" allUniqueName="[Job Shipments].[Ship Dates Match?].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[State Abbr]" caption="State Abbr" attribute="1" defaultMemberUniqueName="[Job Shipments].[State Abbr].[All]" allUniqueName="[Job Shipments].[State Abbr].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Structure Shipment]" caption="Structure Shipment" attribute="1" defaultMemberUniqueName="[Job Shipments].[Structure Shipment].[All]" allUniqueName="[Job Shipments].[Structure Shipment].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Yard Setup]" caption="Yard Setup" attribute="1" defaultMemberUniqueName="[Job Shipments].[Yard Setup].[All]" allUniqueName="[Job Shipments].[Yard Setup].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[Yard Setup Desc]" caption="Yard Setup Desc" attribute="1" defaultMemberUniqueName="[Job Shipments].[Yard Setup Desc].[All]" allUniqueName="[Job Shipments].[Yard Setup Desc].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[HD?]" caption="HD?" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD?].[All]" allUniqueName="[Late End Schedule].[HD?].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[SAP?]" caption="SAP?" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP?].[All]" allUniqueName="[Late End Schedule].[SAP?].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[Task Code]" caption="Task Code" attribute="1" defaultMemberUniqueName="[Late End Schedule].[Task Code].[All]" allUniqueName="[Late End Schedule].[Task Code].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[Task Name]" caption="Task Name" attribute="1" defaultMemberUniqueName="[Late End Schedule].[Task Name].[All]" allUniqueName="[Late End Schedule].[Task Name].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[Task Name Short]" caption="Task Name Short" attribute="1" defaultMemberUniqueName="[Late End Schedule].[Task Name Short].[All]" allUniqueName="[Late End Schedule].[Task Name Short].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[WORK_DAY]" caption="WORK_DAY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[WORK_DAY].[All]" allUniqueName="[Late End Schedule].[WORK_DAY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[Fab Start Date?]" caption="Fab Start Date?" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Fab Start Date?].[All]" allUniqueName="[Milestone Schedule].[Fab Start Date?].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone]" caption="Milestone" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone].[All]" allUniqueName="[Milestone Schedule].[Milestone].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Complete?]" caption="Milestone Complete?" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Complete?].[All]" allUniqueName="[Milestone Schedule].[Milestone Complete?].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Group]" caption="Milestone Group" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Group].[All]" allUniqueName="[Milestone Schedule].[Milestone Group].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Overdue?]" caption="Milestone Overdue?" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Overdue?].[All]" allUniqueName="[Milestone Schedule].[Milestone Overdue?].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Status]" caption="Milestone Status" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Status].[All]" allUniqueName="[Milestone Schedule].[Milestone Status].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[Original Date]" caption="Original Date" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Original Date].[All]" allUniqueName="[Milestone Schedule].[Original Date].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product Groups].[Product Group]" caption="Product Group" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group].[All]" allUniqueName="[Product Groups].[Product Group].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product Groups].[Product Group Desc]" caption="Product Group Desc" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Desc].[All]" allUniqueName="[Product Groups].[Product Group Desc].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product Groups].[Product Group Display]" caption="Product Group Display" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Display].[All]" allUniqueName="[Product Groups].[Product Group Display].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Products].[Product Code]" caption="Product Code" attribute="1" defaultMemberUniqueName="[Products].[Product Code].[All]" allUniqueName="[Products].[Product Code].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Products].[Product Description]" caption="Product Description" attribute="1" defaultMemberUniqueName="[Products].[Product Description].[All]" allUniqueName="[Products].[Product Description].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Products].[Product Display]" caption="Product Display" attribute="1" defaultMemberUniqueName="[Products].[Product Display].[All]" allUniqueName="[Products].[Product Display].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Schedule].[Finish Date Mismatch]" caption="Finish Date Mismatch" attribute="1" defaultMemberUniqueName="[Schedule].[Finish Date Mismatch].[All]" allUniqueName="[Schedule].[Finish Date Mismatch].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Schedule].[HD?]" caption="HD?" attribute="1" defaultMemberUniqueName="[Schedule].[HD?].[All]" allUniqueName="[Schedule].[HD?].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Schedule].[SAP?]" caption="SAP?" attribute="1" defaultMemberUniqueName="[Schedule].[SAP?].[All]" allUniqueName="[Schedule].[SAP?].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Schedule].[Start Date Mismatch]" caption="Start Date Mismatch" attribute="1" defaultMemberUniqueName="[Schedule].[Start Date Mismatch].[All]" allUniqueName="[Schedule].[Start Date Mismatch].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Schedule].[Task Code]" caption="Task Code" attribute="1" defaultMemberUniqueName="[Schedule].[Task Code].[All]" allUniqueName="[Schedule].[Task Code].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Schedule].[Task Name]" caption="Task Name" attribute="1" defaultMemberUniqueName="[Schedule].[Task Name].[All]" allUniqueName="[Schedule].[Task Name].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Schedule].[Task Name Short]" caption="Task Name Short" attribute="1" defaultMemberUniqueName="[Schedule].[Task Name Short].[All]" allUniqueName="[Schedule].[Task Name Short].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Schedule].[Task Start Date]" caption="Task Start Date" attribute="1" defaultMemberUniqueName="[Schedule].[Task Start Date].[All]" allUniqueName="[Schedule].[Task Start Date].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Cost Center Distinct].[COST_CENTER]" caption="COST_CENTER" attribute="1" defaultMemberUniqueName="[Cost Center Distinct].[COST_CENTER].[All]" allUniqueName="[Cost Center Distinct].[COST_CENTER].[All]" dimensionUniqueName="[Cost Center Distinct]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cost Center MPS].[CO_VERSION_ID]" caption="CO_VERSION_ID" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[CO_VERSION_ID].[All]" allUniqueName="[Cost Center MPS].[CO_VERSION_ID].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cost Center MPS].[COST_CENTER]" caption="COST_CENTER" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[COST_CENTER].[All]" allUniqueName="[Cost Center MPS].[COST_CENTER].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cost Center MPS].[DIRECT_MPS]" caption="DIRECT_MPS" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[DIRECT_MPS].[All]" allUniqueName="[Cost Center MPS].[DIRECT_MPS].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cost Center MPS].[EARNED_MPS]" caption="EARNED_MPS" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[EARNED_MPS].[All]" allUniqueName="[Cost Center MPS].[EARNED_MPS].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cost Center MPS].[INDIRECT_MPS]" caption="INDIRECT_MPS" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[INDIRECT_MPS].[All]" allUniqueName="[Cost Center MPS].[INDIRECT_MPS].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cost Center MPS].[OT_MPS]" caption="OT_MPS" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[OT_MPS].[All]" allUniqueName="[Cost Center MPS].[OT_MPS].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cost Center MPS].[WORKDAY_DATE]" caption="WORKDAY_DATE" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[WORKDAY_DATE].[All]" allUniqueName="[Cost Center MPS].[WORKDAY_DATE].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Cost Centers].[COST_CENTER_KEY]" caption="COST_CENTER_KEY" attribute="1" defaultMemberUniqueName="[Cost Centers].[COST_CENTER_KEY].[All]" allUniqueName="[Cost Centers].[COST_CENTER_KEY].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Functions].[FUNCTION_GROUP_SORT]" caption="FUNCTION_GROUP_SORT" attribute="1" defaultMemberUniqueName="[Functions].[FUNCTION_GROUP_SORT].[All]" allUniqueName="[Functions].[FUNCTION_GROUP_SORT].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[COST_CENTER_KEY]" caption="COST_CENTER_KEY" attribute="1" defaultMemberUniqueName="[HD Schedule].[COST_CENTER_KEY].[All]" allUniqueName="[HD Schedule].[COST_CENTER_KEY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HD_HRS_ACTUAL]" caption="DAILY_HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HD_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[DAILY_HD_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HD_HRS_EARNED]" caption="DAILY_HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HD_HRS_EARNED].[All]" allUniqueName="[HD Schedule].[DAILY_HD_HRS_EARNED].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HD_HRS_REMAINING]" caption="DAILY_HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HD_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[DAILY_HD_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HRS_ACTUAL]" caption="DAILY_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[DAILY_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HRS_CURR_EST]" caption="DAILY_HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HRS_CURR_EST].[All]" allUniqueName="[HD Schedule].[DAILY_HRS_CURR_EST].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HRS_REMAINING]" caption="DAILY_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[DAILY_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HRS_TARGET]" caption="DAILY_HRS_TARGET" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HRS_TARGET].[All]" allUniqueName="[HD Schedule].[DAILY_HRS_TARGET].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_SAP_HRS_ACTUAL]" caption="DAILY_SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_SAP_HRS_EARNED]" caption="DAILY_SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_SAP_HRS_EARNED].[All]" allUniqueName="[HD Schedule].[DAILY_SAP_HRS_EARNED].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_SAP_HRS_PLAN]" caption="DAILY_SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_SAP_HRS_PLAN].[All]" allUniqueName="[HD Schedule].[DAILY_SAP_HRS_PLAN].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_SAP_HRS_REMAINING]" caption="DAILY_SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_SAP_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[DAILY_SAP_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[Function Group]" caption="Function Group" attribute="1" defaultMemberUniqueName="[HD Schedule].[Function Group].[All]" allUniqueName="[HD Schedule].[Function Group].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[FUNCTION_CD]" caption="FUNCTION_CD" attribute="1" defaultMemberUniqueName="[HD Schedule].[FUNCTION_CD].[All]" allUniqueName="[HD Schedule].[FUNCTION_CD].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[FUNCTION_GROUP_SORT]" caption="FUNCTION_GROUP_SORT" attribute="1" defaultMemberUniqueName="[HD Schedule].[FUNCTION_GROUP_SORT].[All]" allUniqueName="[HD Schedule].[FUNCTION_GROUP_SORT].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[HD_FINISH_DATE]" caption="HD_FINISH_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_FINISH_DATE].[All]" allUniqueName="[HD Schedule].[HD_FINISH_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[HD_FLAG]" caption="HD_FLAG" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_FLAG].[All]" allUniqueName="[HD Schedule].[HD_FLAG].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[HD_HRS_ACTUAL]" caption="HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[HD_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[HD_HRS_EARNED]" caption="HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_HRS_EARNED].[All]" allUniqueName="[HD Schedule].[HD_HRS_EARNED].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[HD_HRS_REMAINING]" caption="HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[HD_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[HRS_CURR_EST]" caption="HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[HD Schedule].[HRS_CURR_EST].[All]" allUniqueName="[HD Schedule].[HRS_CURR_EST].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[P6_EARLY_END_DATE]" caption="P6_EARLY_END_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_EARLY_END_DATE].[All]" allUniqueName="[HD Schedule].[P6_EARLY_END_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[P6_EARLY_START_DATE]" caption="P6_EARLY_START_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_EARLY_START_DATE].[All]" allUniqueName="[HD Schedule].[P6_EARLY_START_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[P6_END_DATE]" caption="P6_END_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_END_DATE].[All]" allUniqueName="[HD Schedule].[P6_END_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[P6_LATE_END_DATE]" caption="P6_LATE_END_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_LATE_END_DATE].[All]" allUniqueName="[HD Schedule].[P6_LATE_END_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[P6_LATE_START_DATE]" caption="P6_LATE_START_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_LATE_START_DATE].[All]" allUniqueName="[HD Schedule].[P6_LATE_START_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[P6_START_DATE]" caption="P6_START_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_START_DATE].[All]" allUniqueName="[HD Schedule].[P6_START_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[PROD_GRP]" caption="PROD_GRP" attribute="1" defaultMemberUniqueName="[HD Schedule].[PROD_GRP].[All]" allUniqueName="[HD Schedule].[PROD_GRP].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[PRODUCT_CD_SHORT]" caption="PRODUCT_CD_SHORT" attribute="1" defaultMemberUniqueName="[HD Schedule].[PRODUCT_CD_SHORT].[All]" allUniqueName="[HD Schedule].[PRODUCT_CD_SHORT].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[PROJ_SHORT_NAME]" caption="PROJ_SHORT_NAME" attribute="1" defaultMemberUniqueName="[HD Schedule].[PROJ_SHORT_NAME].[All]" allUniqueName="[HD Schedule].[PROJ_SHORT_NAME].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[QTY_ACTUAL]" caption="QTY_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[QTY_ACTUAL].[All]" allUniqueName="[HD Schedule].[QTY_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[QTY_CURR_EST]" caption="QTY_CURR_EST" attribute="1" defaultMemberUniqueName="[HD Schedule].[QTY_CURR_EST].[All]" allUniqueName="[HD Schedule].[QTY_CURR_EST].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[QTY_ROLLUP_KEY]" caption="QTY_ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[HD Schedule].[QTY_ROLLUP_KEY].[All]" allUniqueName="[HD Schedule].[QTY_ROLLUP_KEY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[ROLLUP_KEY]" caption="ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[HD Schedule].[ROLLUP_KEY].[All]" allUniqueName="[HD Schedule].[ROLLUP_KEY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[SAP_FINISH_DATE]" caption="SAP_FINISH_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_FINISH_DATE].[All]" allUniqueName="[HD Schedule].[SAP_FINISH_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[SAP_FLAG]" caption="SAP_FLAG" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_FLAG].[All]" allUniqueName="[HD Schedule].[SAP_FLAG].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[SAP_HRS_ACTUAL]" caption="SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[SAP_HRS_EARNED]" caption="SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_HRS_EARNED].[All]" allUniqueName="[HD Schedule].[SAP_HRS_EARNED].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[SAP_HRS_PLAN]" caption="SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_HRS_PLAN].[All]" allUniqueName="[HD Schedule].[SAP_HRS_PLAN].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[SAP_HRS_REMAINING]" caption="SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[SAP_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[SAP_QTY]" caption="SAP_QTY" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_QTY].[All]" allUniqueName="[HD Schedule].[SAP_QTY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[SAP_QTY_COMPLETE]" caption="SAP_QTY_COMPLETE" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_QTY_COMPLETE].[All]" allUniqueName="[HD Schedule].[SAP_QTY_COMPLETE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[SAP_START_DATE]" caption="SAP_START_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_START_DATE].[All]" allUniqueName="[HD Schedule].[SAP_START_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[TARGET_WORK_QTY]" caption="TARGET_WORK_QTY" attribute="1" defaultMemberUniqueName="[HD Schedule].[TARGET_WORK_QTY].[All]" allUniqueName="[HD Schedule].[TARGET_WORK_QTY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[WORK_DAY]" caption="WORK_DAY" attribute="1" defaultMemberUniqueName="[HD Schedule].[WORK_DAY].[All]" allUniqueName="[HD Schedule].[WORK_DAY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[HD Schedule].[WORK_DAY_COUNT]" caption="WORK_DAY_COUNT" attribute="1" defaultMemberUniqueName="[HD Schedule].[WORK_DAY_COUNT].[All]" allUniqueName="[HD Schedule].[WORK_DAY_COUNT].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[LAST_UPDATED]" caption="LAST_UPDATED" attribute="1" defaultMemberUniqueName="[Job Shipments].[LAST_UPDATED].[All]" allUniqueName="[Job Shipments].[LAST_UPDATED].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[PROJ_ID]" caption="PROJ_ID" attribute="1" defaultMemberUniqueName="[Job Shipments].[PROJ_ID].[All]" allUniqueName="[Job Shipments].[PROJ_ID].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Job Shipments].[SHIP_DATES_DIFF]" caption="SHIP_DATES_DIFF" attribute="1" defaultMemberUniqueName="[Job Shipments].[SHIP_DATES_DIFF].[All]" allUniqueName="[Job Shipments].[SHIP_DATES_DIFF].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[BAY]" caption="BAY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[BAY].[All]" allUniqueName="[Late End Schedule].[BAY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[COST_CENTER]" caption="COST_CENTER" attribute="1" defaultMemberUniqueName="[Late End Schedule].[COST_CENTER].[All]" allUniqueName="[Late End Schedule].[COST_CENTER].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[COST_CENTER_DESC]" caption="COST_CENTER_DESC" attribute="1" defaultMemberUniqueName="[Late End Schedule].[COST_CENTER_DESC].[All]" allUniqueName="[Late End Schedule].[COST_CENTER_DESC].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[COST_CENTER_KEY]" caption="COST_CENTER_KEY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[COST_CENTER_KEY].[All]" allUniqueName="[Late End Schedule].[COST_CENTER_KEY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HD_HRS_ACTUAL]" caption="DAILY_HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HD_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[DAILY_HD_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HD_HRS_EARNED]" caption="DAILY_HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HD_HRS_EARNED].[All]" allUniqueName="[Late End Schedule].[DAILY_HD_HRS_EARNED].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HD_HRS_REMAINING]" caption="DAILY_HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HD_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[DAILY_HD_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HRS_ACTUAL]" caption="DAILY_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[DAILY_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HRS_CURR_EST]" caption="DAILY_HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HRS_CURR_EST].[All]" allUniqueName="[Late End Schedule].[DAILY_HRS_CURR_EST].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HRS_REMAINING]" caption="DAILY_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[DAILY_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HRS_TARGET]" caption="DAILY_HRS_TARGET" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HRS_TARGET].[All]" allUniqueName="[Late End Schedule].[DAILY_HRS_TARGET].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_SAP_HRS_ACTUAL]" caption="DAILY_SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_SAP_HRS_EARNED]" caption="DAILY_SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_SAP_HRS_EARNED].[All]" allUniqueName="[Late End Schedule].[DAILY_SAP_HRS_EARNED].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_SAP_HRS_PLAN]" caption="DAILY_SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_SAP_HRS_PLAN].[All]" allUniqueName="[Late End Schedule].[DAILY_SAP_HRS_PLAN].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_SAP_HRS_REMAINING]" caption="DAILY_SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_SAP_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[DAILY_SAP_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[FINISH_DATE_MISMATCH]" caption="FINISH_DATE_MISMATCH" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FINISH_DATE_MISMATCH].[All]" allUniqueName="[Late End Schedule].[FINISH_DATE_MISMATCH].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[FUNCTION_CD]" caption="FUNCTION_CD" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FUNCTION_CD].[All]" allUniqueName="[Late End Schedule].[FUNCTION_CD].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[FUNCTION_DESC]" caption="FUNCTION_DESC" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FUNCTION_DESC].[All]" allUniqueName="[Late End Schedule].[FUNCTION_DESC].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[FUNCTION_GROUP]" caption="FUNCTION_GROUP" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FUNCTION_GROUP].[All]" allUniqueName="[Late End Schedule].[FUNCTION_GROUP].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[FUNCTION_GROUP_SORT]" caption="FUNCTION_GROUP_SORT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FUNCTION_GROUP_SORT].[All]" allUniqueName="[Late End Schedule].[FUNCTION_GROUP_SORT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[HD_FINISH_DATE]" caption="HD_FINISH_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_FINISH_DATE].[All]" allUniqueName="[Late End Schedule].[HD_FINISH_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[HD_HRS_ACTUAL]" caption="HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[HD_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[HD_HRS_EARNED]" caption="HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_HRS_EARNED].[All]" allUniqueName="[Late End Schedule].[HD_HRS_EARNED].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[HD_HRS_REMAINING]" caption="HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[HD_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[HD_RESOURCE]" caption="HD_RESOURCE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_RESOURCE].[All]" allUniqueName="[Late End Schedule].[HD_RESOURCE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[HD_START_DATE]" caption="HD_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_START_DATE].[All]" allUniqueName="[Late End Schedule].[HD_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[HEIGHT]" caption="HEIGHT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HEIGHT].[All]" allUniqueName="[Late End Schedule].[HEIGHT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[HRS_CURR_EST]" caption="HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HRS_CURR_EST].[All]" allUniqueName="[Late End Schedule].[HRS_CURR_EST].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[LENGTH]" caption="LENGTH" attribute="1" defaultMemberUniqueName="[Late End Schedule].[LENGTH].[All]" allUniqueName="[Late End Schedule].[LENGTH].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[P6_EARLY_END_DATE]" caption="P6_EARLY_END_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_EARLY_END_DATE].[All]" allUniqueName="[Late End Schedule].[P6_EARLY_END_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[P6_EARLY_START_DATE]" caption="P6_EARLY_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_EARLY_START_DATE].[All]" allUniqueName="[Late End Schedule].[P6_EARLY_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[P6_END_DATE]" caption="P6_END_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_END_DATE].[All]" allUniqueName="[Late End Schedule].[P6_END_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[P6_LATE_END_DATE]" caption="P6_LATE_END_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_LATE_END_DATE].[All]" allUniqueName="[Late End Schedule].[P6_LATE_END_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[P6_LATE_START_DATE]" caption="P6_LATE_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_LATE_START_DATE].[All]" allUniqueName="[Late End Schedule].[P6_LATE_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[P6_SHIP_DATE]" caption="P6_SHIP_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_SHIP_DATE].[All]" allUniqueName="[Late End Schedule].[P6_SHIP_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[P6_SHIP_MONTH_YEAR]" caption="P6_SHIP_MONTH_YEAR" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_SHIP_MONTH_YEAR].[All]" allUniqueName="[Late End Schedule].[P6_SHIP_MONTH_YEAR].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[P6_SHIP_YEAR_MONTH]" caption="P6_SHIP_YEAR_MONTH" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_SHIP_YEAR_MONTH].[All]" allUniqueName="[Late End Schedule].[P6_SHIP_YEAR_MONTH].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[P6_START_DATE]" caption="P6_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_START_DATE].[All]" allUniqueName="[Late End Schedule].[P6_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[PLANT]" caption="PLANT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PLANT].[All]" allUniqueName="[Late End Schedule].[PLANT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[PLANT_ID]" caption="PLANT_ID" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PLANT_ID].[All]" allUniqueName="[Late End Schedule].[PLANT_ID].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[PROD_GRP]" caption="PROD_GRP" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PROD_GRP].[All]" allUniqueName="[Late End Schedule].[PROD_GRP].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[PROD_GRP_DESC]" caption="PROD_GRP_DESC" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PROD_GRP_DESC].[All]" allUniqueName="[Late End Schedule].[PROD_GRP_DESC].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[PRODUCT_CD]" caption="PRODUCT_CD" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PRODUCT_CD].[All]" allUniqueName="[Late End Schedule].[PRODUCT_CD].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[PRODUCT_CD_SHORT]" caption="PRODUCT_CD_SHORT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PRODUCT_CD_SHORT].[All]" allUniqueName="[Late End Schedule].[PRODUCT_CD_SHORT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[PROJ_ID]" caption="PROJ_ID" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PROJ_ID].[All]" allUniqueName="[Late End Schedule].[PROJ_ID].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[PROJ_SHORT_NAME]" caption="PROJ_SHORT_NAME" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PROJ_SHORT_NAME].[All]" allUniqueName="[Late End Schedule].[PROJ_SHORT_NAME].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[QTY_ACTUAL]" caption="QTY_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[QTY_ACTUAL].[All]" allUniqueName="[Late End Schedule].[QTY_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[QTY_CURR_EST]" caption="QTY_CURR_EST" attribute="1" defaultMemberUniqueName="[Late End Schedule].[QTY_CURR_EST].[All]" allUniqueName="[Late End Schedule].[QTY_CURR_EST].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[QTY_ROLLUP_KEY]" caption="QTY_ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[QTY_ROLLUP_KEY].[All]" allUniqueName="[Late End Schedule].[QTY_ROLLUP_KEY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[ROLLUP_KEY]" caption="ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[ROLLUP_KEY].[All]" allUniqueName="[Late End Schedule].[ROLLUP_KEY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_FINISH_DATE]" caption="SAP_FINISH_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_FINISH_DATE].[All]" allUniqueName="[Late End Schedule].[SAP_FINISH_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_HRS_ACTUAL]" caption="SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_HRS_EARNED]" caption="SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_HRS_EARNED].[All]" allUniqueName="[Late End Schedule].[SAP_HRS_EARNED].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_HRS_PLAN]" caption="SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_HRS_PLAN].[All]" allUniqueName="[Late End Schedule].[SAP_HRS_PLAN].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_HRS_REMAINING]" caption="SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[SAP_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_QTY]" caption="SAP_QTY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_QTY].[All]" allUniqueName="[Late End Schedule].[SAP_QTY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_QTY_COMPLETE]" caption="SAP_QTY_COMPLETE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_QTY_COMPLETE].[All]" allUniqueName="[Late End Schedule].[SAP_QTY_COMPLETE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_START_DATE]" caption="SAP_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_START_DATE].[All]" allUniqueName="[Late End Schedule].[SAP_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[START_DATE_MISMATCH]" caption="START_DATE_MISMATCH" attribute="1" defaultMemberUniqueName="[Late End Schedule].[START_DATE_MISMATCH].[All]" allUniqueName="[Late End Schedule].[START_DATE_MISMATCH].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[TARGET_WORK_QTY]" caption="TARGET_WORK_QTY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[TARGET_WORK_QTY].[All]" allUniqueName="[Late End Schedule].[TARGET_WORK_QTY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[WORK_CENTER]" caption="WORK_CENTER" attribute="1" defaultMemberUniqueName="[Late End Schedule].[WORK_CENTER].[All]" allUniqueName="[Late End Schedule].[WORK_CENTER].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[WORK_CENTER_DESC]" caption="WORK_CENTER_DESC" attribute="1" defaultMemberUniqueName="[Late End Schedule].[WORK_CENTER_DESC].[All]" allUniqueName="[Late End Schedule].[WORK_CENTER_DESC].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Late End Schedule].[WORK_DAY_COUNT]" caption="WORK_DAY_COUNT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[WORK_DAY_COUNT].[All]" allUniqueName="[Late End Schedule].[WORK_DAY_COUNT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Measures].[COLUMN1]" caption="COLUMN1" attribute="1" defaultMemberUniqueName="[Milestone Measures].[COLUMN1].[All]" allUniqueName="[Milestone Measures].[COLUMN1].[All]" dimensionUniqueName="[Milestone Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Measures].[COLUMN2]" caption="COLUMN2" attribute="1" defaultMemberUniqueName="[Milestone Measures].[COLUMN2].[All]" allUniqueName="[Milestone Measures].[COLUMN2].[All]" dimensionUniqueName="[Milestone Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Measures].[COLUMN3]" caption="COLUMN3" attribute="1" defaultMemberUniqueName="[Milestone Measures].[COLUMN3].[All]" allUniqueName="[Milestone Measures].[COLUMN3].[All]" dimensionUniqueName="[Milestone Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[ACTUAL_DATE]" caption="ACTUAL_DATE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[ACTUAL_DATE].[All]" allUniqueName="[Milestone Schedule].[ACTUAL_DATE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[DAYS_OUT]" caption="DAYS_OUT" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[DAYS_OUT].[All]" allUniqueName="[Milestone Schedule].[DAYS_OUT].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[DUE_DATE]" caption="DUE_DATE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[DUE_DATE].[All]" allUniqueName="[Milestone Schedule].[DUE_DATE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[MATL_MISSING]" caption="MATL_MISSING" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[MATL_MISSING].[All]" allUniqueName="[Milestone Schedule].[MATL_MISSING].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[MILESTONE_GROUP_SORT]" caption="MILESTONE_GROUP_SORT" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[MILESTONE_GROUP_SORT].[All]" allUniqueName="[Milestone Schedule].[MILESTONE_GROUP_SORT].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[MILESTONE_SORT]" caption="MILESTONE_SORT" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[MILESTONE_SORT].[All]" allUniqueName="[Milestone Schedule].[MILESTONE_SORT].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[MILESTONE_STATUS_VALUE]" caption="MILESTONE_STATUS_VALUE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[MILESTONE_STATUS_VALUE].[All]" allUniqueName="[Milestone Schedule].[MILESTONE_STATUS_VALUE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[ORDER_QTY]" caption="ORDER_QTY" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[ORDER_QTY].[All]" allUniqueName="[Milestone Schedule].[ORDER_QTY].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[P6_PROJ_SHORT_NAME]" caption="P6_PROJ_SHORT_NAME" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[P6_PROJ_SHORT_NAME].[All]" allUniqueName="[Milestone Schedule].[P6_PROJ_SHORT_NAME].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[PLOT_DUE_DATE]" caption="PLOT_DUE_DATE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[PLOT_DUE_DATE].[All]" allUniqueName="[Milestone Schedule].[PLOT_DUE_DATE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[QTY_RECVD]" caption="QTY_RECVD" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[QTY_RECVD].[All]" allUniqueName="[Milestone Schedule].[QTY_RECVD].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Milestone Schedule].[REFERENCE_DATE]" caption="REFERENCE_DATE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[REFERENCE_DATE].[All]" allUniqueName="[Milestone Schedule].[REFERENCE_DATE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Public Schedule Measures].[COLUMN1]" caption="COLUMN1" attribute="1" defaultMemberUniqueName="[Public Schedule Measures].[COLUMN1].[All]" allUniqueName="[Public Schedule Measures].[COLUMN1].[All]" dimensionUniqueName="[Public Schedule Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Public Schedule Measures].[COLUMN2]" caption="COLUMN2" attribute="1" defaultMemberUniqueName="[Public Schedule Measures].[COLUMN2].[All]" allUniqueName="[Public Schedule Measures].[COLUMN2].[All]" dimensionUniqueName="[Public Schedule Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Public Schedule Measures].[COLUMN3]" caption="COLUMN3" attribute="1" defaultMemberUniqueName="[Public Schedule Measures].[COLUMN3].[All]" allUniqueName="[Public Schedule Measures].[COLUMN3].[All]" dimensionUniqueName="[Public Schedule Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[BAY]" caption="BAY" attribute="1" defaultMemberUniqueName="[Schedule].[BAY].[All]" allUniqueName="[Schedule].[BAY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[COST_CENTER]" caption="COST_CENTER" attribute="1" defaultMemberUniqueName="[Schedule].[COST_CENTER].[All]" allUniqueName="[Schedule].[COST_CENTER].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[COST_CENTER_DESC]" caption="COST_CENTER_DESC" attribute="1" defaultMemberUniqueName="[Schedule].[COST_CENTER_DESC].[All]" allUniqueName="[Schedule].[COST_CENTER_DESC].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[COST_CENTER_KEY]" caption="COST_CENTER_KEY" attribute="1" defaultMemberUniqueName="[Schedule].[COST_CENTER_KEY].[All]" allUniqueName="[Schedule].[COST_CENTER_KEY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_HD_HRS_ACTUAL]" caption="DAILY_HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HD_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[DAILY_HD_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_HD_HRS_EARNED]" caption="DAILY_HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HD_HRS_EARNED].[All]" allUniqueName="[Schedule].[DAILY_HD_HRS_EARNED].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_HD_HRS_REMAINING]" caption="DAILY_HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HD_HRS_REMAINING].[All]" allUniqueName="[Schedule].[DAILY_HD_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_HRS_ACTUAL]" caption="DAILY_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[DAILY_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_HRS_CURR_EST]" caption="DAILY_HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HRS_CURR_EST].[All]" allUniqueName="[Schedule].[DAILY_HRS_CURR_EST].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_HRS_REMAINING]" caption="DAILY_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HRS_REMAINING].[All]" allUniqueName="[Schedule].[DAILY_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_HRS_TARGET]" caption="DAILY_HRS_TARGET" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HRS_TARGET].[All]" allUniqueName="[Schedule].[DAILY_HRS_TARGET].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_SAP_HRS_ACTUAL]" caption="DAILY_SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_SAP_HRS_EARNED]" caption="DAILY_SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_SAP_HRS_EARNED].[All]" allUniqueName="[Schedule].[DAILY_SAP_HRS_EARNED].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_SAP_HRS_PLAN]" caption="DAILY_SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_SAP_HRS_PLAN].[All]" allUniqueName="[Schedule].[DAILY_SAP_HRS_PLAN].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[DAILY_SAP_HRS_REMAINING]" caption="DAILY_SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_SAP_HRS_REMAINING].[All]" allUniqueName="[Schedule].[DAILY_SAP_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[Function Group]" caption="Function Group" attribute="1" defaultMemberUniqueName="[Schedule].[Function Group].[All]" allUniqueName="[Schedule].[Function Group].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[FUNCTION_CD]" caption="FUNCTION_CD" attribute="1" defaultMemberUniqueName="[Schedule].[FUNCTION_CD].[All]" allUniqueName="[Schedule].[FUNCTION_CD].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[FUNCTION_DESC]" caption="FUNCTION_DESC" attribute="1" defaultMemberUniqueName="[Schedule].[FUNCTION_DESC].[All]" allUniqueName="[Schedule].[FUNCTION_DESC].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[FUNCTION_GROUP_SORT]" caption="FUNCTION_GROUP_SORT" attribute="1" defaultMemberUniqueName="[Schedule].[FUNCTION_GROUP_SORT].[All]" allUniqueName="[Schedule].[FUNCTION_GROUP_SORT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[HD_FINISH_DATE]" caption="HD_FINISH_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[HD_FINISH_DATE].[All]" allUniqueName="[Schedule].[HD_FINISH_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[HD_HRS_ACTUAL]" caption="HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[HD_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[HD_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[HD_HRS_EARNED]" caption="HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Schedule].[HD_HRS_EARNED].[All]" allUniqueName="[Schedule].[HD_HRS_EARNED].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[HD_HRS_REMAINING]" caption="HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[HD_HRS_REMAINING].[All]" allUniqueName="[Schedule].[HD_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[HD_RESOURCE]" caption="HD_RESOURCE" attribute="1" defaultMemberUniqueName="[Schedule].[HD_RESOURCE].[All]" allUniqueName="[Schedule].[HD_RESOURCE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[HD_START_DATE]" caption="HD_START_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[HD_START_DATE].[All]" allUniqueName="[Schedule].[HD_START_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[HEIGHT]" caption="HEIGHT" attribute="1" defaultMemberUniqueName="[Schedule].[HEIGHT].[All]" allUniqueName="[Schedule].[HEIGHT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[HRS_CURR_EST]" caption="HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[Schedule].[HRS_CURR_EST].[All]" allUniqueName="[Schedule].[HRS_CURR_EST].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[LENGTH]" caption="LENGTH" attribute="1" defaultMemberUniqueName="[Schedule].[LENGTH].[All]" allUniqueName="[Schedule].[LENGTH].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[P6_EARLY_END_DATE]" caption="P6_EARLY_END_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_EARLY_END_DATE].[All]" allUniqueName="[Schedule].[P6_EARLY_END_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[P6_END_DATE]" caption="P6_END_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_END_DATE].[All]" allUniqueName="[Schedule].[P6_END_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[P6_LATE_END_DATE]" caption="P6_LATE_END_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_LATE_END_DATE].[All]" allUniqueName="[Schedule].[P6_LATE_END_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[P6_LATE_START_DATE]" caption="P6_LATE_START_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_LATE_START_DATE].[All]" allUniqueName="[Schedule].[P6_LATE_START_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[P6_SHIP_DATE]" caption="P6_SHIP_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_SHIP_DATE].[All]" allUniqueName="[Schedule].[P6_SHIP_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[P6_SHIP_MONTH_YEAR]" caption="P6_SHIP_MONTH_YEAR" attribute="1" defaultMemberUniqueName="[Schedule].[P6_SHIP_MONTH_YEAR].[All]" allUniqueName="[Schedule].[P6_SHIP_MONTH_YEAR].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[P6_SHIP_YEAR_MONTH]" caption="P6_SHIP_YEAR_MONTH" attribute="1" defaultMemberUniqueName="[Schedule].[P6_SHIP_YEAR_MONTH].[All]" allUniqueName="[Schedule].[P6_SHIP_YEAR_MONTH].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[P6_START_DATE]" caption="P6_START_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_START_DATE].[All]" allUniqueName="[Schedule].[P6_START_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[PLANT]" caption="PLANT" attribute="1" defaultMemberUniqueName="[Schedule].[PLANT].[All]" allUniqueName="[Schedule].[PLANT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[PLANT_ID]" caption="PLANT_ID" attribute="1" defaultMemberUniqueName="[Schedule].[PLANT_ID].[All]" allUniqueName="[Schedule].[PLANT_ID].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[PROD_GRP]" caption="PROD_GRP" attribute="1" defaultMemberUniqueName="[Schedule].[PROD_GRP].[All]" allUniqueName="[Schedule].[PROD_GRP].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[PROD_GRP_DESC]" caption="PROD_GRP_DESC" attribute="1" defaultMemberUniqueName="[Schedule].[PROD_GRP_DESC].[All]" allUniqueName="[Schedule].[PROD_GRP_DESC].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[PRODUCT_CD]" caption="PRODUCT_CD" attribute="1" defaultMemberUniqueName="[Schedule].[PRODUCT_CD].[All]" allUniqueName="[Schedule].[PRODUCT_CD].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[PRODUCT_CD_SHORT]" caption="PRODUCT_CD_SHORT" attribute="1" defaultMemberUniqueName="[Schedule].[PRODUCT_CD_SHORT].[All]" allUniqueName="[Schedule].[PRODUCT_CD_SHORT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[PROJ_ID]" caption="PROJ_ID" attribute="1" defaultMemberUniqueName="[Schedule].[PROJ_ID].[All]" allUniqueName="[Schedule].[PROJ_ID].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[PROJ_SHORT_NAME]" caption="PROJ_SHORT_NAME" attribute="1" defaultMemberUniqueName="[Schedule].[PROJ_SHORT_NAME].[All]" allUniqueName="[Schedule].[PROJ_SHORT_NAME].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[QTY_ACTUAL]" caption="QTY_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[QTY_ACTUAL].[All]" allUniqueName="[Schedule].[QTY_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[QTY_CURR_EST]" caption="QTY_CURR_EST" attribute="1" defaultMemberUniqueName="[Schedule].[QTY_CURR_EST].[All]" allUniqueName="[Schedule].[QTY_CURR_EST].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[QTY_ROLLUP_KEY]" caption="QTY_ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[Schedule].[QTY_ROLLUP_KEY].[All]" allUniqueName="[Schedule].[QTY_ROLLUP_KEY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[ROLLUP_KEY]" caption="ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[Schedule].[ROLLUP_KEY].[All]" allUniqueName="[Schedule].[ROLLUP_KEY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[SAP_FINISH_DATE]" caption="SAP_FINISH_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_FINISH_DATE].[All]" allUniqueName="[Schedule].[SAP_FINISH_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[SAP_HRS_ACTUAL]" caption="SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[SAP_HRS_EARNED]" caption="SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_HRS_EARNED].[All]" allUniqueName="[Schedule].[SAP_HRS_EARNED].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[SAP_HRS_PLAN]" caption="SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_HRS_PLAN].[All]" allUniqueName="[Schedule].[SAP_HRS_PLAN].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[SAP_HRS_REMAINING]" caption="SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_HRS_REMAINING].[All]" allUniqueName="[Schedule].[SAP_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[SAP_QTY]" caption="SAP_QTY" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_QTY].[All]" allUniqueName="[Schedule].[SAP_QTY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[SAP_QTY_COMPLETE]" caption="SAP_QTY_COMPLETE" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_QTY_COMPLETE].[All]" allUniqueName="[Schedule].[SAP_QTY_COMPLETE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[SAP_START_DATE]" caption="SAP_START_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_START_DATE].[All]" allUniqueName="[Schedule].[SAP_START_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[TARGET_WORK_QTY]" caption="TARGET_WORK_QTY" attribute="1" defaultMemberUniqueName="[Schedule].[TARGET_WORK_QTY].[All]" allUniqueName="[Schedule].[TARGET_WORK_QTY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[WORK_CENTER]" caption="WORK_CENTER" attribute="1" defaultMemberUniqueName="[Schedule].[WORK_CENTER].[All]" allUniqueName="[Schedule].[WORK_CENTER].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[WORK_CENTER_DESC]" caption="WORK_CENTER_DESC" attribute="1" defaultMemberUniqueName="[Schedule].[WORK_CENTER_DESC].[All]" allUniqueName="[Schedule].[WORK_CENTER_DESC].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[WORK_DAY]" caption="WORK_DAY" attribute="1" defaultMemberUniqueName="[Schedule].[WORK_DAY].[All]" allUniqueName="[Schedule].[WORK_DAY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Schedule].[WORK_DAY_COUNT]" caption="WORK_DAY_COUNT" attribute="1" defaultMemberUniqueName="[Schedule].[WORK_DAY_COUNT].[All]" allUniqueName="[Schedule].[WORK_DAY_COUNT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Scheduling Measures].[COLUMN1]" caption="COLUMN1" attribute="1" defaultMemberUniqueName="[Scheduling Measures].[COLUMN1].[All]" allUniqueName="[Scheduling Measures].[COLUMN1].[All]" dimensionUniqueName="[Scheduling Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Scheduling Measures].[COLUMN2]" caption="COLUMN2" attribute="1" defaultMemberUniqueName="[Scheduling Measures].[COLUMN2].[All]" allUniqueName="[Scheduling Measures].[COLUMN2].[All]" dimensionUniqueName="[Scheduling Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Scheduling Measures].[COLUMN3]" caption="COLUMN3" attribute="1" defaultMemberUniqueName="[Scheduling Measures].[COLUMN3].[All]" allUniqueName="[Scheduling Measures].[COLUMN3].[All]" dimensionUniqueName="[Scheduling Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Milestone Days Out]" caption="Milestone Days Out" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Matl Order Qty]" caption="Matl Order Qty" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Matl Recvd Qty]" caption="Matl Recvd Qty" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Matl Missing Qty]" caption="Matl Missing Qty" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Milestone Due Date]" caption="Milestone Due Date" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Milestone Status Value]" caption="Milestone Status Value" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Milestone Days Overdue]" caption="Milestone Days Overdue" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Milestone Count]" caption="Milestone Count" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Completed Milestones]" caption="Completed Milestones" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Incomplete Milestones]" caption="Incomplete Milestones" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Milestone Group Status]" caption="Milestone Group Status" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Milestone Column Value 2 3]" caption="Milestone Column Value 2 3" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Milestone Column Value 1 4]" caption="Milestone Column Value 1 4" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[P6 Remaining Hours]" caption="P6 Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[P6 Scheduled Remaining Hours]" caption="P6 Scheduled Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD Remaining Hours]" caption="HD Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD Scheduled Remaining Hours]" caption="HD Scheduled Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD Qty]" caption="HD Qty" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD Start Date]" caption="HD Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD End Date]" caption="HD End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Start Date]" caption="SAP Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP End Date]" caption="SAP End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Qty]" caption="SAP Qty" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Qty Complete]" caption="SAP Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Qty Remaining]" caption="SAP Qty Remaining" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Qty % Complete]" caption="SAP Qty % Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Plan Hours]" caption="SAP Plan Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Actual Hours]" caption="SAP Actual Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Earned Hours]" caption="SAP Earned Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Remaining Hours]" caption="SAP Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[SAP Scheduled Remaining Hours]" caption="SAP Scheduled Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[P6 Target Hours]" caption="P6 Target Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Remaining Hours Adjusted]" caption="Remaining Hours Adjusted" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD Earned Hours]" caption="HD Earned Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD Plan Hours]" caption="HD Plan Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD Qty Complete]" caption="HD Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD Qty Remaining]" caption="HD Qty Remaining" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[HD Qty % Complete]" caption="HD Qty % Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Data Last Updated]" caption="Data Last Updated" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Ship Date Status Indicator]" caption="Ship Date Status Indicator" measure="1" displayFolder="Indicators" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Ship Date]" caption="Ship Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Earned MPS (004)]" caption="Earned MPS (004)" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Active Job Remaining Hours]" caption="Active Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Planned Job Remaining Hours]" caption="Planned Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Active Job Start Date]" caption="Active Job Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Planned Job Start Date]" caption="Planned Job Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Job Status Indicator]" caption="Job Status Indicator" measure="1" displayFolder="Indicators" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[What-If Job Remaining Hours]" caption="What-If Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Inactive Job Remaining Hours]" caption="Inactive Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[P6 Girder Start Date]" caption="P6 Girder Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[P6 Early Start Date]" caption="P6 Early Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[P6 Early End Date]" caption="P6 Early End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Fab Start Date]" caption="Fab Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Fab End Date]" caption="Fab End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Yard Start Date]" caption="Yard Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Yard End Date]" caption="Yard End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Coatings Start Date]" caption="Coatings Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Coatings End Date]" caption="Coatings End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[P6 Late Remaining Hours]" caption="P6 Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Active Job Late Remaining Hours]" caption="Active Job Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Planned Job Late Remaining Hours]" caption="Planned Job Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[What-If Job Late Remaining Hours]" caption="What-If Job Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Inactive Job Late Remaining Hours]" caption="Inactive Job Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Remaining Hours]" caption="Public Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Active Job Remaining Hours]" caption="Public Active Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Planned Job Remaining Hours]" caption="Public Planned Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Start Date]" caption="Public Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public End Date]" caption="Public End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public HD Qty]" caption="Public HD Qty" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public HD Qty Complete]" caption="Public HD Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public HD Qty Remaining]" caption="Public HD Qty Remaining" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public HD Qty % Complete]" caption="Public HD Qty % Complete" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Girder Start Date]" caption="Public Girder Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public What-If Job Remaining Hours]" caption="Public What-If Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Inactive Job Remaining Hours]" caption="Public Inactive Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Fab Start Date]" caption="Public Fab Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Fab End Date]" caption="Public Fab End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Yard Start Date]" caption="Public Yard Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Yard End Date]" caption="Public Yard End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Coatings Start Date]" caption="Public Coatings Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Coatings End Date]" caption="Public Coatings End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Average Days Out]" caption="Average Days Out" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[P6 End Date]" caption="P6 End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Avg HD Qty]" caption="Avg HD Qty" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Avg SAP Qty]" caption="Avg SAP Qty" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Avg SAP Qty Complete]" caption="Avg SAP Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Avg HD Qty Complete]" caption="Avg HD Qty Complete" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Bay Schedule 2 and 3 Export Link]" caption="Bay Schedule 2 and 3 Export Link" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Bay Schedule 1 and 4 Export Link]" caption="Bay Schedule 1 and 4 Export Link" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Bay Schedule 2 and 3 Export Link MS]" caption="Bay Schedule 2 and 3 Export Link MS" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Bay Schedule 1 and 4 Export Link MS]" caption="Bay Schedule 1 and 4 Export Link MS" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Early Start Date Export Link]" caption="Early Start Date Export Link" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Early Start Date Export Link MS]" caption="Early Start Date Export Link MS" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Avg HD Qty]" caption="Public Avg HD Qty" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Avg HD Qty Complete]" caption="Public Avg HD Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0" hidden="1"/>
+    <cacheHierarchy uniqueName="[Measures].[__Default measure]" caption="__Default measure" measure="1" displayFolder="" count="0" hidden="1"/>
+  </cacheHierarchies>
+  <kpis count="0"/>
+  <dimensions count="11">
+    <dimension name="Calendar" uniqueName="[Calendar]" caption="Calendar"/>
+    <dimension name="Cost Centers" uniqueName="[Cost Centers]" caption="Cost Centers"/>
+    <dimension name="Functions" uniqueName="[Functions]" caption="Functions"/>
+    <dimension name="HD Schedule" uniqueName="[HD Schedule]" caption="HD Schedule"/>
+    <dimension name="Job Shipments" uniqueName="[Job Shipments]" caption="Job Shipments"/>
+    <dimension name="Late End Schedule" uniqueName="[Late End Schedule]" caption="Late End Schedule"/>
+    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
+    <dimension name="Milestone Schedule" uniqueName="[Milestone Schedule]" caption="Milestone Schedule"/>
+    <dimension name="Product Groups" uniqueName="[Product Groups]" caption="Product Groups"/>
+    <dimension name="Products" uniqueName="[Products]" caption="Products"/>
+    <dimension name="Schedule" uniqueName="[Schedule]" caption="Schedule"/>
+  </dimensions>
+  <measureGroups count="15">
+    <measureGroup name="Calendar" caption="Calendar"/>
+    <measureGroup name="Cost Center Distinct" caption="Cost Center Distinct"/>
+    <measureGroup name="Cost Center MPS" caption="Cost Center MPS"/>
+    <measureGroup name="Cost Centers" caption="Cost Centers"/>
+    <measureGroup name="Functions" caption="Functions"/>
+    <measureGroup name="HD Schedule" caption="HD Schedule"/>
+    <measureGroup name="Job Shipments" caption="Job Shipments"/>
+    <measureGroup name="Late End Schedule" caption="Late End Schedule"/>
+    <measureGroup name="Milestone Measures" caption="Milestone Measures"/>
+    <measureGroup name="Milestone Schedule" caption="Milestone Schedule"/>
+    <measureGroup name="Product Groups" caption="Product Groups"/>
+    <measureGroup name="Products" caption="Products"/>
+    <measureGroup name="Public Schedule Measures" caption="Public Schedule Measures"/>
+    <measureGroup name="Schedule" caption="Schedule"/>
+    <measureGroup name="Scheduling Measures" caption="Scheduling Measures"/>
+  </measureGroups>
+  <maps count="10">
+    <map measureGroup="0" dimension="0"/>
+    <map measureGroup="3" dimension="1"/>
+    <map measureGroup="4" dimension="2"/>
+    <map measureGroup="5" dimension="3"/>
+    <map measureGroup="6" dimension="4"/>
+    <map measureGroup="7" dimension="5"/>
+    <map measureGroup="9" dimension="7"/>
+    <map measureGroup="10" dimension="8"/>
+    <map measureGroup="11" dimension="9"/>
+    <map measureGroup="13" dimension="10"/>
+  </maps>
+  <extLst>
+    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
+      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
+    </ext>
+  </extLst>
+</pivotCacheDefinition>
+</file>
+
+<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43984.290081250001" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+  <cacheSource type="external" connectionId="1"/>
+  <cacheFields count="4">
+    <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
+      <sharedItems count="199">
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160230F-06]" c="D-1160230F-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160245A-02]" c="D-1160245A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160245A-13]" c="D-1160245A-13"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-01]" c="D-1160253A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-02]" c="D-1160253A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-04]" c="D-1160253C-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-05]" c="D-1160253C-05"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-06]" c="D-1160253C-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-07]" c="D-1160253C-07"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032A-01]" c="D-1170032A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032A-02]" c="D-1170032A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032B-03]" c="D-1170032B-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170082A-03]" c="D-1170082A-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170082D-08]" c="D-1170082D-08"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-02]" c="D-1170143C-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-03]" c="D-1170143C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-04]" c="D-1170143C-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155A-01]" c="D-1170155A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155D-04]" c="D-1170155D-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155G-13]" c="D-1170155G-13"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217A-01]" c="D-1170217A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217C-03]" c="D-1170217C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217F-07]" c="D-1170217F-07"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217G-08]" c="D-1170217G-08"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272A-01]" c="D-1170272A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272B-02]" c="D-1170272B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272C-03]" c="D-1170272C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272E-05]" c="D-1170272E-05"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272F-06]" c="D-1170272F-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272G-07]" c="D-1170272G-07"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170281B-01]" c="D-1170281B-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180020A-01]" c="D-1180020A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180023A-02]" c="D-1180023A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045A-01]" c="D-1180045A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045A-02]" c="D-1180045A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045A-03]" c="D-1180045A-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045B-04]" c="D-1180045B-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045B-05]" c="D-1180045B-05"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045B-06]" c="D-1180045B-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180059A-01]" c="D-1180059A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180059A-02]" c="D-1180059A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180081A-02]" c="D-1180081A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180091C-03]" c="D-1180091C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180091C-04]" c="D-1180091C-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095C-03]" c="D-1180095C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095D-04]" c="D-1180095D-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095D-05]" c="D-1180095D-05"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095E-06]" c="D-1180095E-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095G-08]" c="D-1180095G-08"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095H-09]" c="D-1180095H-09"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095J-10]" c="D-1180095J-10"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095L-12]" c="D-1180095L-12"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180116B-01]" c="D-1180116B-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180136A-01]" c="D-1180136A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180155A-02]" c="D-1180155A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180155A-03]" c="D-1180155A-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180164A-01]" c="D-1180164A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180164A-02]" c="D-1180164A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180174A-02]" c="D-1180174A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201A-01]" c="D-1180201A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201A-02]" c="D-1180201A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201B-03]" c="D-1180201B-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201B-12]" c="D-1180201B-12"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201C-04]" c="D-1180201C-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201C-05]" c="D-1180201C-05"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201C-13]" c="D-1180201C-13"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201D-06]" c="D-1180201D-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201D-07]" c="D-1180201D-07"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201E-08]" c="D-1180201E-08"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201F-09]" c="D-1180201F-09"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201G-10]" c="D-1180201G-10"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201H-11]" c="D-1180201H-11"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238A-01]" c="D-1180238A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238B-02]" c="D-1180238B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238C-03]" c="D-1180238C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238D-04]" c="D-1180238D-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238D-05]" c="D-1180238D-05"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238E-06]" c="D-1180238E-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238E-07]" c="D-1180238E-07"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238F-08]" c="D-1180238F-08"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238G-09]" c="D-1180238G-09"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180246A-01]" c="D-1180246A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-01]" c="D-1180261A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-02]" c="D-1180261A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180262A-02]" c="D-1180262A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180274A-02]" c="D-1180274A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285A-01]" c="D-1180285A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285C-03]" c="D-1180285C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285D-04]" c="D-1180285D-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180302A-01]" c="D-1180302A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180308A-01]" c="D-1180308A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180308A-02]" c="D-1180308A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180308A-03]" c="D-1180308A-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180310A-01]" c="D-1180310A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190010A-01]" c="D-1190010A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190016A-01]" c="D-1190016A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190028A-01]" c="D-1190028A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190028B-02]" c="D-1190028B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190036A-01]" c="D-1190036A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190037A-01]" c="D-1190037A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190038A-01]" c="D-1190038A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190060A-01]" c="D-1190060A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190066A-01]" c="D-1190066A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190078A-01]" c="D-1190078A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190090A-01]" c="D-1190090A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190092A-02]" c="D-1190092A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190092B-04]" c="D-1190092B-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190096A-01]" c="D-1190096A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190102A-01]" c="D-1190102A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190103A-03]" c="D-1190103A-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190103A-04]" c="D-1190103A-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190105A-01]" c="D-1190105A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190105A-02]" c="D-1190105A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190118A-01]" c="D-1190118A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190118A-02]" c="D-1190118A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190118B-03]" c="D-1190118B-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190118B-04]" c="D-1190118B-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190124A-01]" c="D-1190124A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190128A-01]" c="D-1190128A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190128B-02]" c="D-1190128B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190130A-01]" c="D-1190130A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190130B-02]" c="D-1190130B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190135A-01]" c="D-1190135A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190136A-01]" c="D-1190136A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190136A-02]" c="D-1190136A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190138A-01]" c="D-1190138A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190144A-01]" c="D-1190144A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190144B-02]" c="D-1190144B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190145A-01]" c="D-1190145A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190148A-01]" c="D-1190148A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190165A-01]" c="D-1190165A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190179A-01]" c="D-1190179A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190187A-01]" c="D-1190187A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190193A-01]" c="D-1190193A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190196A-01]" c="D-1190196A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190203A-01]" c="D-1190203A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190210A-01]" c="D-1190210A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190214A-01]" c="D-1190214A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190217A-01]" c="D-1190217A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190227A-01]" c="D-1190227A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190230A-01]" c="D-1190230A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190232A-01]" c="D-1190232A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190232B-02]" c="D-1190232B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190232C-03]" c="D-1190232C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190239A-01]" c="D-1190239A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190243A-01]" c="D-1190243A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190243B-02]" c="D-1190243B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190249A-01]" c="D-1190249A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190249B-02]" c="D-1190249B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250A-01]" c="D-1190250A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250A-02]" c="D-1190250A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250A-03]" c="D-1190250A-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250B-04]" c="D-1190250B-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250B-05]" c="D-1190250B-05"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250B-06]" c="D-1190250B-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250C-07]" c="D-1190250C-07"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250D-08]" c="D-1190250D-08"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250E-09]" c="D-1190250E-09"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190251B-02]" c="D-1190251B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190254A-01]" c="D-1190254A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190258A-01]" c="D-1190258A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190259A-01]" c="D-1190259A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190259A-02]" c="D-1190259A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190259A-03]" c="D-1190259A-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190266A-01]" c="D-1190266A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190272A-01]" c="D-1190272A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190272B-02]" c="D-1190272B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274A-01]" c="D-1190274A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274B-02]" c="D-1190274B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278A-01]" c="D-1190278A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278B-02]" c="D-1190278B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278C-03]" c="D-1190278C-03"/>
@@ -955,42 +1656,29 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200021A-01]" c="D-1200021A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200023A-01]" c="D-1200023A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200031A-01]" c="D-1200031A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200034A-01]" c="D-1200034A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200089A-03]" c="D-1200089A-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160230F-06]" u="1" c="D-1160230F-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-02]" u="1" c="D-1160253A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-06]" u="1" c="D-1160253C-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-07]" u="1" c="D-1160253C-07"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-03]" u="1" c="D-1170143C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-04]" u="1" c="D-1170143C-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155A-01]" u="1" c="D-1170155A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155G-13]" u="1" c="D-1170155G-13"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217G-08]" u="1" c="D-1170217G-08"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095C-03]" u="1" c="D-1180095C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095J-10]" u="1" c="D-1180095J-10"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238A-01]" u="1" c="D-1180238A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238B-02]" u="1" c="D-1180238B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238C-03]" u="1" c="D-1180238C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238G-09]" u="1" c="D-1180238G-09"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-01]" u="1" c="D-1180261A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-02]" u="1" c="D-1180261A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180262A-02]" u="1" c="D-1180262A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190037A-01]" u="1" c="D-1190037A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190145A-01]" u="1" c="D-1190145A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190187A-01]" u="1" c="D-1190187A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274B-02]" u="1" c="D-1190274B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200034A-01]" u="1" c="D-1200034A-01"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Products].[Product Code].[Product Code]" caption="Product Code" numFmtId="0" hierarchy="79" level="1">
-      <sharedItems count="5">
-        <s v="[Products].[Product Code].&amp;[G]" c="G"/>
-        <s v="[Products].[Product Code].&amp;[BG]" c="BG"/>
-        <s v="[Products].[Product Code].&amp;[S]" c="S"/>
-        <s v="[Products].[Product Code].&amp;[TG]" c="TG"/>
-        <s v="[Products].[Product Code].&amp;[PD]" c="PD"/>
       </sharedItems>
     </cacheField>
     <cacheField name="[Measures].[Public Start Date]" caption="Public Start Date" numFmtId="0" hierarchy="360" level="32767"/>
+    <cacheField name="[Measures].[Public Girder Start Date]" caption="Public Girder Start Date" numFmtId="0" hierarchy="366" level="32767"/>
+    <cacheField name="[Product Groups].[Product Group Desc].[Product Group Desc]" caption="Product Group Desc" numFmtId="0" hierarchy="77" level="1">
+      <sharedItems count="13">
+        <s v="[Product Groups].[Product Group Desc].&amp;[Misc]" c="Misc"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Parts]" c="Parts"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Shapes]" c="Shapes"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Bearings]" c="Bearings"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Box Girders]" c="Box Girders"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Cross Frames]" c="Cross Frames"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Diaphragms]" c="Diaphragms"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Girders]" c="Girders"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Lateral Bracing]" c="Lateral Bracing"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Other]" c="Other"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Plate Diaphragms]" c="Plate Diaphragms"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Stringers]" c="Stringers"/>
+        <s v="[Product Groups].[Product Group Desc].&amp;[Tub Girders]" c="Tub Girders"/>
+      </sharedItems>
+    </cacheField>
   </cacheFields>
   <cacheHierarchies count="390">
     <cacheHierarchy uniqueName="[Calendar].[Calendar Date]" caption="Calendar Date" attribute="1" defaultMemberUniqueName="[Calendar].[Calendar Date].[All]" allUniqueName="[Calendar].[Calendar Date].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
@@ -1075,14 +1763,14 @@
     <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Status]" caption="Milestone Status" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Status].[All]" allUniqueName="[Milestone Schedule].[Milestone Status].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Milestone Schedule].[Original Date]" caption="Original Date" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Original Date].[All]" allUniqueName="[Milestone Schedule].[Original Date].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Product Groups].[Product Group]" caption="Product Group" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group].[All]" allUniqueName="[Product Groups].[Product Group].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product Groups].[Product Group Desc]" caption="Product Group Desc" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Desc].[All]" allUniqueName="[Product Groups].[Product Group Desc].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product Groups].[Product Group Display]" caption="Product Group Display" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Display].[All]" allUniqueName="[Product Groups].[Product Group Display].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Products].[Product Code]" caption="Product Code" attribute="1" defaultMemberUniqueName="[Products].[Product Code].[All]" allUniqueName="[Products].[Product Code].[All]" dimensionUniqueName="[Products]" displayFolder="" count="2" unbalanced="0">
+    <cacheHierarchy uniqueName="[Product Groups].[Product Group Desc]" caption="Product Group Desc" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Desc].[All]" allUniqueName="[Product Groups].[Product Group Desc].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
+        <fieldUsage x="3"/>
       </fieldsUsage>
     </cacheHierarchy>
+    <cacheHierarchy uniqueName="[Product Groups].[Product Group Display]" caption="Product Group Display" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Display].[All]" allUniqueName="[Product Groups].[Product Group Display].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Products].[Product Code]" caption="Product Code" attribute="1" defaultMemberUniqueName="[Products].[Product Code].[All]" allUniqueName="[Products].[Product Code].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Product Description]" caption="Product Description" attribute="1" defaultMemberUniqueName="[Products].[Product Description].[All]" allUniqueName="[Products].[Product Description].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Product Display]" caption="Product Display" attribute="1" defaultMemberUniqueName="[Products].[Product Display].[All]" allUniqueName="[Products].[Product Display].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Schedule].[Finish Date Mismatch]" caption="Finish Date Mismatch" attribute="1" defaultMemberUniqueName="[Schedule].[Finish Date Mismatch].[All]" allUniqueName="[Schedule].[Finish Date Mismatch].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
@@ -1365,7 +2053,7 @@
     <cacheHierarchy uniqueName="[Measures].[Public Planned Job Remaining Hours]" caption="Public Planned Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Public Start Date]" caption="Public Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0" oneField="1">
       <fieldsUsage count="1">
-        <fieldUsage x="2"/>
+        <fieldUsage x="1"/>
       </fieldsUsage>
     </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Public End Date]" caption="Public End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
@@ -1373,7 +2061,11 @@
     <cacheHierarchy uniqueName="[Measures].[Public HD Qty Complete]" caption="Public HD Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Public HD Qty Remaining]" caption="Public HD Qty Remaining" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Public HD Qty % Complete]" caption="Public HD Qty % Complete" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Girder Start Date]" caption="Public Girder Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
+    <cacheHierarchy uniqueName="[Measures].[Public Girder Start Date]" caption="Public Girder Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0" oneField="1">
+      <fieldsUsage count="1">
+        <fieldUsage x="2"/>
+      </fieldsUsage>
+    </cacheHierarchy>
     <cacheHierarchy uniqueName="[Measures].[Public What-If Job Remaining Hours]" caption="Public What-If Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Public Inactive Job Remaining Hours]" caption="Public Inactive Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Public Fab Start Date]" caption="Public Fab Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
@@ -1449,8 +2141,8 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43983.633052083336" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
+<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43984.290084722219" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
@@ -2138,36 +2830,27 @@
 </pivotCacheDefinition>
 </file>
 
-<file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43983.633056944447" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43984.290088078706" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
   <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="4">
+  <cacheFields count="3">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
       <sharedItems count="199">
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160230F-06]" c="D-1160230F-06"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160245A-02]" c="D-1160245A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160245A-13]" c="D-1160245A-13"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-01]" c="D-1160253A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-02]" c="D-1160253A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-04]" c="D-1160253C-04"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-05]" c="D-1160253C-05"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-06]" c="D-1160253C-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-07]" c="D-1160253C-07"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032A-01]" c="D-1170032A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032A-02]" c="D-1170032A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032B-03]" c="D-1170032B-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170082A-03]" c="D-1170082A-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170082D-08]" c="D-1170082D-08"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-02]" c="D-1170143C-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-03]" c="D-1170143C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-04]" c="D-1170143C-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155A-01]" c="D-1170155A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155D-04]" c="D-1170155D-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155G-13]" c="D-1170155G-13"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217A-01]" c="D-1170217A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217C-03]" c="D-1170217C-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217F-07]" c="D-1170217F-07"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217G-08]" c="D-1170217G-08"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272A-01]" c="D-1170272A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272B-02]" c="D-1170272B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272C-03]" c="D-1170272C-03"/>
@@ -2188,13 +2871,11 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180081A-02]" c="D-1180081A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180091C-03]" c="D-1180091C-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180091C-04]" c="D-1180091C-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095C-03]" c="D-1180095C-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095D-04]" c="D-1180095D-04"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095D-05]" c="D-1180095D-05"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095E-06]" c="D-1180095E-06"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095G-08]" c="D-1180095G-08"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095H-09]" c="D-1180095H-09"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095J-10]" c="D-1180095J-10"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095L-12]" c="D-1180095L-12"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180116B-01]" c="D-1180116B-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180136A-01]" c="D-1180136A-01"/>
@@ -2216,19 +2897,12 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201F-09]" c="D-1180201F-09"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201G-10]" c="D-1180201G-10"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201H-11]" c="D-1180201H-11"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238A-01]" c="D-1180238A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238B-02]" c="D-1180238B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238C-03]" c="D-1180238C-03"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238D-04]" c="D-1180238D-04"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238D-05]" c="D-1180238D-05"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238E-06]" c="D-1180238E-06"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238E-07]" c="D-1180238E-07"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238F-08]" c="D-1180238F-08"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238G-09]" c="D-1180238G-09"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180246A-01]" c="D-1180246A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-01]" c="D-1180261A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-02]" c="D-1180261A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180262A-02]" c="D-1180262A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180274A-02]" c="D-1180274A-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285A-01]" c="D-1180285A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285C-03]" c="D-1180285C-03"/>
@@ -2243,7 +2917,6 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190028A-01]" c="D-1190028A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190028B-02]" c="D-1190028B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190036A-01]" c="D-1190036A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190037A-01]" c="D-1190037A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190038A-01]" c="D-1190038A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190060A-01]" c="D-1190060A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190066A-01]" c="D-1190066A-01"/>
@@ -2272,11 +2945,9 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190138A-01]" c="D-1190138A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190144A-01]" c="D-1190144A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190144B-02]" c="D-1190144B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190145A-01]" c="D-1190145A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190148A-01]" c="D-1190148A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190165A-01]" c="D-1190165A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190179A-01]" c="D-1190179A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190187A-01]" c="D-1190187A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190193A-01]" c="D-1190193A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190196A-01]" c="D-1190196A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190203A-01]" c="D-1190203A-01"/>
@@ -2312,7 +2983,6 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190272A-01]" c="D-1190272A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190272B-02]" c="D-1190272B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274A-01]" c="D-1190274A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274B-02]" c="D-1190274B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278A-01]" c="D-1190278A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278B-02]" c="D-1190278B-02"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278C-03]" c="D-1190278C-03"/>
@@ -2341,29 +3011,42 @@
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200021A-01]" c="D-1200021A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200023A-01]" c="D-1200023A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200031A-01]" c="D-1200031A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200034A-01]" c="D-1200034A-01"/>
         <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200089A-03]" c="D-1200089A-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160230F-06]" u="1" c="D-1160230F-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-02]" u="1" c="D-1160253A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-06]" u="1" c="D-1160253C-06"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-07]" u="1" c="D-1160253C-07"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-03]" u="1" c="D-1170143C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-04]" u="1" c="D-1170143C-04"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155A-01]" u="1" c="D-1170155A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155G-13]" u="1" c="D-1170155G-13"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217G-08]" u="1" c="D-1170217G-08"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095C-03]" u="1" c="D-1180095C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095J-10]" u="1" c="D-1180095J-10"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238A-01]" u="1" c="D-1180238A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238B-02]" u="1" c="D-1180238B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238C-03]" u="1" c="D-1180238C-03"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238G-09]" u="1" c="D-1180238G-09"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-01]" u="1" c="D-1180261A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-02]" u="1" c="D-1180261A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180262A-02]" u="1" c="D-1180262A-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190037A-01]" u="1" c="D-1190037A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190145A-01]" u="1" c="D-1190145A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190187A-01]" u="1" c="D-1190187A-01"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274B-02]" u="1" c="D-1190274B-02"/>
+        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200034A-01]" u="1" c="D-1200034A-01"/>
+      </sharedItems>
+    </cacheField>
+    <cacheField name="[Products].[Product Code].[Product Code]" caption="Product Code" numFmtId="0" hierarchy="79" level="1">
+      <sharedItems count="5">
+        <s v="[Products].[Product Code].&amp;[G]" c="G"/>
+        <s v="[Products].[Product Code].&amp;[BG]" c="BG"/>
+        <s v="[Products].[Product Code].&amp;[S]" c="S"/>
+        <s v="[Products].[Product Code].&amp;[TG]" c="TG"/>
+        <s v="[Products].[Product Code].&amp;[PD]" c="PD"/>
       </sharedItems>
     </cacheField>
     <cacheField name="[Measures].[Public Start Date]" caption="Public Start Date" numFmtId="0" hierarchy="360" level="32767"/>
-    <cacheField name="[Measures].[Public Girder Start Date]" caption="Public Girder Start Date" numFmtId="0" hierarchy="366" level="32767"/>
-    <cacheField name="[Product Groups].[Product Group Desc].[Product Group Desc]" caption="Product Group Desc" numFmtId="0" hierarchy="77" level="1">
-      <sharedItems count="13">
-        <s v="[Product Groups].[Product Group Desc].&amp;[Misc]" c="Misc"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Parts]" c="Parts"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Shapes]" c="Shapes"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Bearings]" c="Bearings"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Box Girders]" c="Box Girders"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Cross Frames]" c="Cross Frames"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Diaphragms]" c="Diaphragms"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Girders]" c="Girders"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Lateral Bracing]" c="Lateral Bracing"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Other]" c="Other"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Plate Diaphragms]" c="Plate Diaphragms"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Stringers]" c="Stringers"/>
-        <s v="[Product Groups].[Product Group Desc].&amp;[Tub Girders]" c="Tub Girders"/>
-      </sharedItems>
-    </cacheField>
   </cacheFields>
   <cacheHierarchies count="390">
     <cacheHierarchy uniqueName="[Calendar].[Calendar Date]" caption="Calendar Date" attribute="1" defaultMemberUniqueName="[Calendar].[Calendar Date].[All]" allUniqueName="[Calendar].[Calendar Date].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
@@ -2448,14 +3131,14 @@
     <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Status]" caption="Milestone Status" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Status].[All]" allUniqueName="[Milestone Schedule].[Milestone Status].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Milestone Schedule].[Original Date]" caption="Original Date" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Original Date].[All]" allUniqueName="[Milestone Schedule].[Original Date].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Product Groups].[Product Group]" caption="Product Group" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group].[All]" allUniqueName="[Product Groups].[Product Group].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product Groups].[Product Group Desc]" caption="Product Group Desc" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Desc].[All]" allUniqueName="[Product Groups].[Product Group Desc].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="2" unbalanced="0">
+    <cacheHierarchy uniqueName="[Product Groups].[Product Group Desc]" caption="Product Group Desc" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Desc].[All]" allUniqueName="[Product Groups].[Product Group Desc].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Product Groups].[Product Group Display]" caption="Product Group Display" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Display].[All]" allUniqueName="[Product Groups].[Product Group Display].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
+    <cacheHierarchy uniqueName="[Products].[Product Code]" caption="Product Code" attribute="1" defaultMemberUniqueName="[Products].[Product Code].[All]" allUniqueName="[Products].[Product Code].[All]" dimensionUniqueName="[Products]" displayFolder="" count="2" unbalanced="0">
       <fieldsUsage count="2">
         <fieldUsage x="-1"/>
-        <fieldUsage x="3"/>
+        <fieldUsage x="1"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Product Groups].[Product Group Display]" caption="Product Group Display" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Display].[All]" allUniqueName="[Product Groups].[Product Group Display].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Products].[Product Code]" caption="Product Code" attribute="1" defaultMemberUniqueName="[Products].[Product Code].[All]" allUniqueName="[Products].[Product Code].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Product Description]" caption="Product Description" attribute="1" defaultMemberUniqueName="[Products].[Product Description].[All]" allUniqueName="[Products].[Product Description].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Products].[Product Display]" caption="Product Display" attribute="1" defaultMemberUniqueName="[Products].[Product Display].[All]" allUniqueName="[Products].[Product Display].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
     <cacheHierarchy uniqueName="[Schedule].[Finish Date Mismatch]" caption="Finish Date Mismatch" attribute="1" defaultMemberUniqueName="[Schedule].[Finish Date Mismatch].[All]" allUniqueName="[Schedule].[Finish Date Mismatch].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
@@ -2738,686 +3421,9 @@
     <cacheHierarchy uniqueName="[Measures].[Public Planned Job Remaining Hours]" caption="Public Planned Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Public Start Date]" caption="Public Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0" oneField="1">
       <fieldsUsage count="1">
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Public End Date]" caption="Public End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public HD Qty]" caption="Public HD Qty" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public HD Qty Complete]" caption="Public HD Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public HD Qty Remaining]" caption="Public HD Qty Remaining" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public HD Qty % Complete]" caption="Public HD Qty % Complete" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Girder Start Date]" caption="Public Girder Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0" oneField="1">
-      <fieldsUsage count="1">
         <fieldUsage x="2"/>
       </fieldsUsage>
     </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Measures].[Public What-If Job Remaining Hours]" caption="Public What-If Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Inactive Job Remaining Hours]" caption="Public Inactive Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Fab Start Date]" caption="Public Fab Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Fab End Date]" caption="Public Fab End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Yard Start Date]" caption="Public Yard Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Yard End Date]" caption="Public Yard End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Coatings Start Date]" caption="Public Coatings Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Coatings End Date]" caption="Public Coatings End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Average Days Out]" caption="Average Days Out" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[P6 End Date]" caption="P6 End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Avg HD Qty]" caption="Avg HD Qty" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Avg SAP Qty]" caption="Avg SAP Qty" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Avg SAP Qty Complete]" caption="Avg SAP Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Avg HD Qty Complete]" caption="Avg HD Qty Complete" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Bay Schedule 2 and 3 Export Link]" caption="Bay Schedule 2 and 3 Export Link" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Bay Schedule 1 and 4 Export Link]" caption="Bay Schedule 1 and 4 Export Link" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Bay Schedule 2 and 3 Export Link MS]" caption="Bay Schedule 2 and 3 Export Link MS" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Bay Schedule 1 and 4 Export Link MS]" caption="Bay Schedule 1 and 4 Export Link MS" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Early Start Date Export Link]" caption="Early Start Date Export Link" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Early Start Date Export Link MS]" caption="Early Start Date Export Link MS" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Avg HD Qty]" caption="Public Avg HD Qty" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Avg HD Qty Complete]" caption="Public Avg HD Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[__Default measure]" caption="__Default measure" measure="1" displayFolder="" count="0" hidden="1"/>
-  </cacheHierarchies>
-  <kpis count="0"/>
-  <dimensions count="11">
-    <dimension name="Calendar" uniqueName="[Calendar]" caption="Calendar"/>
-    <dimension name="Cost Centers" uniqueName="[Cost Centers]" caption="Cost Centers"/>
-    <dimension name="Functions" uniqueName="[Functions]" caption="Functions"/>
-    <dimension name="HD Schedule" uniqueName="[HD Schedule]" caption="HD Schedule"/>
-    <dimension name="Job Shipments" uniqueName="[Job Shipments]" caption="Job Shipments"/>
-    <dimension name="Late End Schedule" uniqueName="[Late End Schedule]" caption="Late End Schedule"/>
-    <dimension measure="1" name="Measures" uniqueName="[Measures]" caption="Measures"/>
-    <dimension name="Milestone Schedule" uniqueName="[Milestone Schedule]" caption="Milestone Schedule"/>
-    <dimension name="Product Groups" uniqueName="[Product Groups]" caption="Product Groups"/>
-    <dimension name="Products" uniqueName="[Products]" caption="Products"/>
-    <dimension name="Schedule" uniqueName="[Schedule]" caption="Schedule"/>
-  </dimensions>
-  <measureGroups count="15">
-    <measureGroup name="Calendar" caption="Calendar"/>
-    <measureGroup name="Cost Center Distinct" caption="Cost Center Distinct"/>
-    <measureGroup name="Cost Center MPS" caption="Cost Center MPS"/>
-    <measureGroup name="Cost Centers" caption="Cost Centers"/>
-    <measureGroup name="Functions" caption="Functions"/>
-    <measureGroup name="HD Schedule" caption="HD Schedule"/>
-    <measureGroup name="Job Shipments" caption="Job Shipments"/>
-    <measureGroup name="Late End Schedule" caption="Late End Schedule"/>
-    <measureGroup name="Milestone Measures" caption="Milestone Measures"/>
-    <measureGroup name="Milestone Schedule" caption="Milestone Schedule"/>
-    <measureGroup name="Product Groups" caption="Product Groups"/>
-    <measureGroup name="Products" caption="Products"/>
-    <measureGroup name="Public Schedule Measures" caption="Public Schedule Measures"/>
-    <measureGroup name="Schedule" caption="Schedule"/>
-    <measureGroup name="Scheduling Measures" caption="Scheduling Measures"/>
-  </measureGroups>
-  <maps count="10">
-    <map measureGroup="0" dimension="0"/>
-    <map measureGroup="3" dimension="1"/>
-    <map measureGroup="4" dimension="2"/>
-    <map measureGroup="5" dimension="3"/>
-    <map measureGroup="6" dimension="4"/>
-    <map measureGroup="7" dimension="5"/>
-    <map measureGroup="9" dimension="7"/>
-    <map measureGroup="10" dimension="8"/>
-    <map measureGroup="11" dimension="9"/>
-    <map measureGroup="13" dimension="10"/>
-  </maps>
-  <extLst>
-    <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{725AE2AE-9491-48be-B2B4-4EB974FC3084}">
-      <x14:pivotCacheDefinition supportSubqueryNonVisual="1" supportSubqueryCalcMem="1" supportAddCalcMems="1"/>
-    </ext>
-  </extLst>
-</pivotCacheDefinition>
-</file>
-
-<file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43983.633061574074" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
-  <cacheSource type="external" connectionId="1"/>
-  <cacheFields count="2">
-    <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
-      <sharedItems count="200">
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160230F-06]" c="D-1160230F-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160245A-02]" c="D-1160245A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160245A-13]" c="D-1160245A-13"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-01]" c="D-1160253A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253A-02]" c="D-1160253A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-04]" c="D-1160253C-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-05]" c="D-1160253C-05"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-06]" c="D-1160253C-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1160253C-07]" c="D-1160253C-07"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032A-01]" c="D-1170032A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032A-02]" c="D-1170032A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170032B-03]" c="D-1170032B-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170082A-03]" c="D-1170082A-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170082D-08]" c="D-1170082D-08"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-02]" c="D-1170143C-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-03]" c="D-1170143C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170143C-04]" c="D-1170143C-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155A-01]" c="D-1170155A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155D-04]" c="D-1170155D-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170155G-13]" c="D-1170155G-13"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217A-01]" c="D-1170217A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217C-03]" c="D-1170217C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217F-07]" c="D-1170217F-07"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170217G-08]" c="D-1170217G-08"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272A-01]" c="D-1170272A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272B-02]" c="D-1170272B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272C-03]" c="D-1170272C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272E-05]" c="D-1170272E-05"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272F-06]" c="D-1170272F-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170272G-07]" c="D-1170272G-07"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1170281B-01]" c="D-1170281B-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180020A-01]" c="D-1180020A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180023A-02]" c="D-1180023A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045A-01]" c="D-1180045A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045A-02]" c="D-1180045A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045A-03]" c="D-1180045A-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045B-04]" c="D-1180045B-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045B-05]" c="D-1180045B-05"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180045B-06]" c="D-1180045B-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180059A-01]" c="D-1180059A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180059A-02]" c="D-1180059A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180081A-02]" c="D-1180081A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180091C-03]" c="D-1180091C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180091C-04]" c="D-1180091C-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095C-03]" c="D-1180095C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095D-04]" c="D-1180095D-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095D-05]" c="D-1180095D-05"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095E-06]" c="D-1180095E-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095G-08]" c="D-1180095G-08"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095H-09]" c="D-1180095H-09"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095J-10]" c="D-1180095J-10"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180095L-12]" c="D-1180095L-12"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180116B-01]" c="D-1180116B-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180136A-01]" c="D-1180136A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180155A-02]" c="D-1180155A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180155A-03]" c="D-1180155A-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180164A-01]" c="D-1180164A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180164A-02]" c="D-1180164A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180174A-02]" c="D-1180174A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201A-01]" c="D-1180201A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201A-02]" c="D-1180201A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201B-03]" c="D-1180201B-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201B-12]" c="D-1180201B-12"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201C-04]" c="D-1180201C-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201C-05]" c="D-1180201C-05"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201C-13]" c="D-1180201C-13"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201D-06]" c="D-1180201D-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201D-07]" c="D-1180201D-07"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201E-08]" c="D-1180201E-08"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201F-09]" c="D-1180201F-09"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201G-10]" c="D-1180201G-10"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180201H-11]" c="D-1180201H-11"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238A-01]" c="D-1180238A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238B-02]" c="D-1180238B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238C-03]" c="D-1180238C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238D-04]" c="D-1180238D-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238D-05]" c="D-1180238D-05"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238E-06]" c="D-1180238E-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238E-07]" c="D-1180238E-07"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238F-08]" c="D-1180238F-08"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180238G-09]" c="D-1180238G-09"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180246A-01]" c="D-1180246A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-01]" c="D-1180261A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180261A-02]" c="D-1180261A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180262A-02]" c="D-1180262A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180274A-02]" c="D-1180274A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285A-01]" c="D-1180285A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285C-03]" c="D-1180285C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180285D-04]" c="D-1180285D-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180302A-01]" c="D-1180302A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180308A-01]" c="D-1180308A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180308A-02]" c="D-1180308A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180308A-03]" c="D-1180308A-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1180310A-01]" c="D-1180310A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190010A-01]" c="D-1190010A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190016A-01]" c="D-1190016A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190028A-01]" c="D-1190028A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190028B-02]" c="D-1190028B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190036A-01]" c="D-1190036A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190037A-01]" c="D-1190037A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190038A-01]" c="D-1190038A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190060A-01]" c="D-1190060A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190066A-01]" c="D-1190066A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190078A-01]" c="D-1190078A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190090A-01]" c="D-1190090A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190092A-02]" c="D-1190092A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190092B-04]" c="D-1190092B-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190096A-01]" c="D-1190096A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190102A-01]" c="D-1190102A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190103A-03]" c="D-1190103A-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190103A-04]" c="D-1190103A-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190105A-01]" c="D-1190105A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190105A-02]" c="D-1190105A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190118A-01]" c="D-1190118A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190118A-02]" c="D-1190118A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190118B-03]" c="D-1190118B-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190118B-04]" c="D-1190118B-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190124A-01]" c="D-1190124A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190128A-01]" c="D-1190128A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190128B-02]" c="D-1190128B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190130A-01]" c="D-1190130A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190130B-02]" c="D-1190130B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190135A-01]" c="D-1190135A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190136A-01]" c="D-1190136A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190136A-02]" c="D-1190136A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190138A-01]" c="D-1190138A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190144A-01]" c="D-1190144A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190144B-02]" c="D-1190144B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190145A-01]" c="D-1190145A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190148A-01]" c="D-1190148A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190165A-01]" c="D-1190165A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190179A-01]" c="D-1190179A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190187A-01]" c="D-1190187A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190193A-01]" c="D-1190193A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190196A-01]" c="D-1190196A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190203A-01]" c="D-1190203A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190210A-01]" c="D-1190210A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190214A-01]" c="D-1190214A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190217A-01]" c="D-1190217A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190227A-01]" c="D-1190227A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190230A-01]" c="D-1190230A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190232A-01]" c="D-1190232A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190232B-02]" c="D-1190232B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190232C-03]" c="D-1190232C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190239A-01]" c="D-1190239A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190243A-01]" c="D-1190243A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190243B-02]" c="D-1190243B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190249A-01]" c="D-1190249A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190249B-02]" c="D-1190249B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250A-01]" c="D-1190250A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250A-02]" c="D-1190250A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250A-03]" c="D-1190250A-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250B-04]" c="D-1190250B-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250B-05]" c="D-1190250B-05"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250B-06]" c="D-1190250B-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250C-07]" c="D-1190250C-07"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250D-08]" c="D-1190250D-08"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190250E-09]" c="D-1190250E-09"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190251B-02]" c="D-1190251B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190254A-01]" c="D-1190254A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190258A-01]" c="D-1190258A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190259A-01]" c="D-1190259A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190259A-02]" c="D-1190259A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190259A-03]" c="D-1190259A-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190266A-01]" c="D-1190266A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190272A-01]" c="D-1190272A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190272B-02]" c="D-1190272B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274A-01]" c="D-1190274A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190274B-02]" c="D-1190274B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278A-01]" c="D-1190278A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278B-02]" c="D-1190278B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278C-03]" c="D-1190278C-03"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278C-04]" c="D-1190278C-04"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278C-05]" c="D-1190278C-05"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278D-06]" c="D-1190278D-06"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278D-07]" c="D-1190278D-07"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278E-08]" c="D-1190278E-08"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278E-09]" c="D-1190278E-09"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278F-10]" c="D-1190278F-10"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190278G-11]" c="D-1190278G-11"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190279A-01]" c="D-1190279A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190283A-01]" c="D-1190283A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190289A-01]" c="D-1190289A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190295A-01]" c="D-1190295A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190300A-01]" c="D-1190300A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190305A-01]" c="D-1190305A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190306A-01]" c="D-1190306A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190310A-01]" c="D-1190310A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190310B-02]" c="D-1190310B-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190320A-01]" c="D-1190320A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1190321A-01]" c="D-1190321A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200014A-01]" c="D-1200014A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200017A-01]" c="D-1200017A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200017A-02]" c="D-1200017A-02"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200021A-01]" c="D-1200021A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200022A-01]" c="D-1200022A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200023A-01]" c="D-1200023A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200031A-01]" c="D-1200031A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200034A-01]" c="D-1200034A-01"/>
-        <s v="[Job Shipments].[Job Structure Shipment].&amp;[D-1200089A-03]" c="D-1200089A-03"/>
-      </sharedItems>
-    </cacheField>
-    <cacheField name="[Job Shipments].[PM Initials].[PM Initials]" caption="PM Initials" numFmtId="0" hierarchy="50" level="1">
-      <sharedItems count="7">
-        <s v="[Job Shipments].[PM Initials].&amp;[MK]" c="MK"/>
-        <s v="[Job Shipments].[PM Initials].&amp;[DP]" c="DP"/>
-        <s v="[Job Shipments].[PM Initials].&amp;[JF]" c="JF"/>
-        <s v="[Job Shipments].[PM Initials].&amp;[JW]" c="JW"/>
-        <s v="[Job Shipments].[PM Initials].&amp;[KG]" c="KG"/>
-        <s v="[Job Shipments].[PM Initials].&amp;[MD]" c="MD"/>
-        <s v="[Job Shipments].[PM Initials].&amp;" c=""/>
-      </sharedItems>
-    </cacheField>
-  </cacheFields>
-  <cacheHierarchies count="390">
-    <cacheHierarchy uniqueName="[Calendar].[Calendar Date]" caption="Calendar Date" attribute="1" defaultMemberUniqueName="[Calendar].[Calendar Date].[All]" allUniqueName="[Calendar].[Calendar Date].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Month Ending]" caption="Month Ending" attribute="1" defaultMemberUniqueName="[Calendar].[Month Ending].[All]" allUniqueName="[Calendar].[Month Ending].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Month Name]" caption="Month Name" attribute="1" defaultMemberUniqueName="[Calendar].[Month Name].[All]" allUniqueName="[Calendar].[Month Name].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Month Number]" caption="Month Number" attribute="1" defaultMemberUniqueName="[Calendar].[Month Number].[All]" allUniqueName="[Calendar].[Month Number].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Month Short Name]" caption="Month Short Name" attribute="1" defaultMemberUniqueName="[Calendar].[Month Short Name].[All]" allUniqueName="[Calendar].[Month Short Name].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Month Starting]" caption="Month Starting" attribute="1" defaultMemberUniqueName="[Calendar].[Month Starting].[All]" allUniqueName="[Calendar].[Month Starting].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Month Year]" caption="Month Year" attribute="1" defaultMemberUniqueName="[Calendar].[Month Year].[All]" allUniqueName="[Calendar].[Month Year].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Months Out]" caption="Months Out" attribute="1" defaultMemberUniqueName="[Calendar].[Months Out].[All]" allUniqueName="[Calendar].[Months Out].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Quarter]" caption="Quarter" attribute="1" defaultMemberUniqueName="[Calendar].[Quarter].[All]" allUniqueName="[Calendar].[Quarter].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Week Beginning]" caption="Week Beginning" attribute="1" defaultMemberUniqueName="[Calendar].[Week Beginning].[All]" allUniqueName="[Calendar].[Week Beginning].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Week Ending]" caption="Week Ending" attribute="1" defaultMemberUniqueName="[Calendar].[Week Ending].[All]" allUniqueName="[Calendar].[Week Ending].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Weeks Out]" caption="Weeks Out" attribute="1" defaultMemberUniqueName="[Calendar].[Weeks Out].[All]" allUniqueName="[Calendar].[Weeks Out].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Year]" caption="Year" attribute="1" defaultMemberUniqueName="[Calendar].[Year].[All]" allUniqueName="[Calendar].[Year].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Year Month]" caption="Year Month" attribute="1" defaultMemberUniqueName="[Calendar].[Year Month].[All]" allUniqueName="[Calendar].[Year Month].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Calendar].[Year Qtr]" caption="Year Qtr" attribute="1" defaultMemberUniqueName="[Calendar].[Year Qtr].[All]" allUniqueName="[Calendar].[Year Qtr].[All]" dimensionUniqueName="[Calendar]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[Bay]" caption="Bay" attribute="1" defaultMemberUniqueName="[Cost Centers].[Bay].[All]" allUniqueName="[Cost Centers].[Bay].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[Cost Center]" caption="Cost Center" attribute="1" defaultMemberUniqueName="[Cost Centers].[Cost Center].[All]" allUniqueName="[Cost Centers].[Cost Center].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[Cost Center Display]" caption="Cost Center Display" attribute="1" defaultMemberUniqueName="[Cost Centers].[Cost Center Display].[All]" allUniqueName="[Cost Centers].[Cost Center Display].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[Cost Center Name]" caption="Cost Center Name" attribute="1" defaultMemberUniqueName="[Cost Centers].[Cost Center Name].[All]" allUniqueName="[Cost Centers].[Cost Center Name].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[Facility]" caption="Facility" attribute="1" defaultMemberUniqueName="[Cost Centers].[Facility].[All]" allUniqueName="[Cost Centers].[Facility].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[Plant]" caption="Plant" attribute="1" defaultMemberUniqueName="[Cost Centers].[Plant].[All]" allUniqueName="[Cost Centers].[Plant].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[Work Center]" caption="Work Center" attribute="1" defaultMemberUniqueName="[Cost Centers].[Work Center].[All]" allUniqueName="[Cost Centers].[Work Center].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[Work Center Display]" caption="Work Center Display" attribute="1" defaultMemberUniqueName="[Cost Centers].[Work Center Display].[All]" allUniqueName="[Cost Centers].[Work Center Display].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[Work Center Name]" caption="Work Center Name" attribute="1" defaultMemberUniqueName="[Cost Centers].[Work Center Name].[All]" allUniqueName="[Cost Centers].[Work Center Name].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Functions].[Function Code]" caption="Function Code" attribute="1" defaultMemberUniqueName="[Functions].[Function Code].[All]" allUniqueName="[Functions].[Function Code].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Functions].[Function Description]" caption="Function Description" attribute="1" defaultMemberUniqueName="[Functions].[Function Description].[All]" allUniqueName="[Functions].[Function Description].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Functions].[Function Display]" caption="Function Display" attribute="1" defaultMemberUniqueName="[Functions].[Function Display].[All]" allUniqueName="[Functions].[Function Display].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Functions].[Function Group]" caption="Function Group" attribute="1" defaultMemberUniqueName="[Functions].[Function Group].[All]" allUniqueName="[Functions].[Function Group].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[Finish Date Mismatch]" caption="Finish Date Mismatch" attribute="1" defaultMemberUniqueName="[HD Schedule].[Finish Date Mismatch].[All]" allUniqueName="[HD Schedule].[Finish Date Mismatch].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[Start Date Mismatch]" caption="Start Date Mismatch" attribute="1" defaultMemberUniqueName="[HD Schedule].[Start Date Mismatch].[All]" allUniqueName="[HD Schedule].[Start Date Mismatch].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[Task Code]" caption="Task Code" attribute="1" defaultMemberUniqueName="[HD Schedule].[Task Code].[All]" allUniqueName="[HD Schedule].[Task Code].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[Task Name]" caption="Task Name" attribute="1" defaultMemberUniqueName="[HD Schedule].[Task Name].[All]" allUniqueName="[HD Schedule].[Task Name].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[Task Name Short]" caption="Task Name Short" attribute="1" defaultMemberUniqueName="[HD Schedule].[Task Name Short].[All]" allUniqueName="[HD Schedule].[Task Name Short].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[Task Start Date]" caption="Task Start Date" attribute="1" defaultMemberUniqueName="[HD Schedule].[Task Start Date].[All]" allUniqueName="[HD Schedule].[Task Start Date].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Coating]" caption="Coating" attribute="1" defaultMemberUniqueName="[Job Shipments].[Coating].[All]" allUniqueName="[Job Shipments].[Coating].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Coating Desc]" caption="Coating Desc" attribute="1" defaultMemberUniqueName="[Job Shipments].[Coating Desc].[All]" allUniqueName="[Job Shipments].[Coating Desc].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Display Ship Date]" caption="Display Ship Date" attribute="1" defaultMemberUniqueName="[Job Shipments].[Display Ship Date].[All]" allUniqueName="[Job Shipments].[Display Ship Date].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[First Start Date]" caption="First Start Date" attribute="1" defaultMemberUniqueName="[Job Shipments].[First Start Date].[All]" allUniqueName="[Job Shipments].[First Start Date].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[HD Ship Date]" caption="HD Ship Date" attribute="1" defaultMemberUniqueName="[Job Shipments].[HD Ship Date].[All]" allUniqueName="[Job Shipments].[HD Ship Date].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[In HD?]" caption="In HD?" attribute="1" defaultMemberUniqueName="[Job Shipments].[In HD?].[All]" allUniqueName="[Job Shipments].[In HD?].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Job Name]" caption="Job Name" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Name].[All]" allUniqueName="[Job Shipments].[Job Name].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Job Number]" caption="Job Number" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Number].[All]" allUniqueName="[Job Shipments].[Job Number].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Job State]" caption="Job State" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job State].[All]" allUniqueName="[Job Shipments].[Job State].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Job Status]" caption="Job Status" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Status].[All]" allUniqueName="[Job Shipments].[Job Status].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Job Status Full Text]" caption="Job Status Full Text" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Status Full Text].[All]" allUniqueName="[Job Shipments].[Job Status Full Text].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Job Structure Shipment]" caption="Job Structure Shipment" attribute="1" defaultMemberUniqueName="[Job Shipments].[Job Structure Shipment].[All]" allUniqueName="[Job Shipments].[Job Structure Shipment].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="0"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Job Shipments].[Milestone Status Text]" caption="Milestone Status Text" attribute="1" defaultMemberUniqueName="[Job Shipments].[Milestone Status Text].[All]" allUniqueName="[Job Shipments].[Milestone Status Text].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[P6 Ship Date]" caption="P6 Ship Date" attribute="1" defaultMemberUniqueName="[Job Shipments].[P6 Ship Date].[All]" allUniqueName="[Job Shipments].[P6 Ship Date].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[P6 Ship Month Year]" caption="P6 Ship Month Year" attribute="1" defaultMemberUniqueName="[Job Shipments].[P6 Ship Month Year].[All]" allUniqueName="[Job Shipments].[P6 Ship Month Year].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[P6 Ship Year Month]" caption="P6 Ship Year Month" attribute="1" defaultMemberUniqueName="[Job Shipments].[P6 Ship Year Month].[All]" allUniqueName="[Job Shipments].[P6 Ship Year Month].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[PM Initials]" caption="PM Initials" attribute="1" defaultMemberUniqueName="[Job Shipments].[PM Initials].[All]" allUniqueName="[Job Shipments].[PM Initials].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="2" unbalanced="0">
-      <fieldsUsage count="2">
-        <fieldUsage x="-1"/>
-        <fieldUsage x="1"/>
-      </fieldsUsage>
-    </cacheHierarchy>
-    <cacheHierarchy uniqueName="[Job Shipments].[Production Status]" caption="Production Status" attribute="1" defaultMemberUniqueName="[Job Shipments].[Production Status].[All]" allUniqueName="[Job Shipments].[Production Status].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Project Manager]" caption="Project Manager" attribute="1" defaultMemberUniqueName="[Job Shipments].[Project Manager].[All]" allUniqueName="[Job Shipments].[Project Manager].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Project Milestone Status]" caption="Project Milestone Status" attribute="1" defaultMemberUniqueName="[Job Shipments].[Project Milestone Status].[All]" allUniqueName="[Job Shipments].[Project Milestone Status].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Project Notes]" caption="Project Notes" attribute="1" defaultMemberUniqueName="[Job Shipments].[Project Notes].[All]" allUniqueName="[Job Shipments].[Project Notes].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Project Ship Date Status]" caption="Project Ship Date Status" attribute="1" defaultMemberUniqueName="[Job Shipments].[Project Ship Date Status].[All]" allUniqueName="[Job Shipments].[Project Ship Date Status].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Ship Date Job Label]" caption="Ship Date Job Label" attribute="1" defaultMemberUniqueName="[Job Shipments].[Ship Date Job Label].[All]" allUniqueName="[Job Shipments].[Ship Date Job Label].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Ship Date Status Text]" caption="Ship Date Status Text" attribute="1" defaultMemberUniqueName="[Job Shipments].[Ship Date Status Text].[All]" allUniqueName="[Job Shipments].[Ship Date Status Text].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Ship Dates Match?]" caption="Ship Dates Match?" attribute="1" defaultMemberUniqueName="[Job Shipments].[Ship Dates Match?].[All]" allUniqueName="[Job Shipments].[Ship Dates Match?].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[State Abbr]" caption="State Abbr" attribute="1" defaultMemberUniqueName="[Job Shipments].[State Abbr].[All]" allUniqueName="[Job Shipments].[State Abbr].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Structure Shipment]" caption="Structure Shipment" attribute="1" defaultMemberUniqueName="[Job Shipments].[Structure Shipment].[All]" allUniqueName="[Job Shipments].[Structure Shipment].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Yard Setup]" caption="Yard Setup" attribute="1" defaultMemberUniqueName="[Job Shipments].[Yard Setup].[All]" allUniqueName="[Job Shipments].[Yard Setup].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[Yard Setup Desc]" caption="Yard Setup Desc" attribute="1" defaultMemberUniqueName="[Job Shipments].[Yard Setup Desc].[All]" allUniqueName="[Job Shipments].[Yard Setup Desc].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[HD?]" caption="HD?" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD?].[All]" allUniqueName="[Late End Schedule].[HD?].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[SAP?]" caption="SAP?" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP?].[All]" allUniqueName="[Late End Schedule].[SAP?].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[Task Code]" caption="Task Code" attribute="1" defaultMemberUniqueName="[Late End Schedule].[Task Code].[All]" allUniqueName="[Late End Schedule].[Task Code].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[Task Name]" caption="Task Name" attribute="1" defaultMemberUniqueName="[Late End Schedule].[Task Name].[All]" allUniqueName="[Late End Schedule].[Task Name].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[Task Name Short]" caption="Task Name Short" attribute="1" defaultMemberUniqueName="[Late End Schedule].[Task Name Short].[All]" allUniqueName="[Late End Schedule].[Task Name Short].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[WORK_DAY]" caption="WORK_DAY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[WORK_DAY].[All]" allUniqueName="[Late End Schedule].[WORK_DAY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[Fab Start Date?]" caption="Fab Start Date?" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Fab Start Date?].[All]" allUniqueName="[Milestone Schedule].[Fab Start Date?].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone]" caption="Milestone" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone].[All]" allUniqueName="[Milestone Schedule].[Milestone].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Complete?]" caption="Milestone Complete?" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Complete?].[All]" allUniqueName="[Milestone Schedule].[Milestone Complete?].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Group]" caption="Milestone Group" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Group].[All]" allUniqueName="[Milestone Schedule].[Milestone Group].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Overdue?]" caption="Milestone Overdue?" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Overdue?].[All]" allUniqueName="[Milestone Schedule].[Milestone Overdue?].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[Milestone Status]" caption="Milestone Status" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Milestone Status].[All]" allUniqueName="[Milestone Schedule].[Milestone Status].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[Original Date]" caption="Original Date" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[Original Date].[All]" allUniqueName="[Milestone Schedule].[Original Date].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product Groups].[Product Group]" caption="Product Group" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group].[All]" allUniqueName="[Product Groups].[Product Group].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product Groups].[Product Group Desc]" caption="Product Group Desc" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Desc].[All]" allUniqueName="[Product Groups].[Product Group Desc].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Product Groups].[Product Group Display]" caption="Product Group Display" attribute="1" defaultMemberUniqueName="[Product Groups].[Product Group Display].[All]" allUniqueName="[Product Groups].[Product Group Display].[All]" dimensionUniqueName="[Product Groups]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Products].[Product Code]" caption="Product Code" attribute="1" defaultMemberUniqueName="[Products].[Product Code].[All]" allUniqueName="[Products].[Product Code].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Products].[Product Description]" caption="Product Description" attribute="1" defaultMemberUniqueName="[Products].[Product Description].[All]" allUniqueName="[Products].[Product Description].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Products].[Product Display]" caption="Product Display" attribute="1" defaultMemberUniqueName="[Products].[Product Display].[All]" allUniqueName="[Products].[Product Display].[All]" dimensionUniqueName="[Products]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Schedule].[Finish Date Mismatch]" caption="Finish Date Mismatch" attribute="1" defaultMemberUniqueName="[Schedule].[Finish Date Mismatch].[All]" allUniqueName="[Schedule].[Finish Date Mismatch].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Schedule].[HD?]" caption="HD?" attribute="1" defaultMemberUniqueName="[Schedule].[HD?].[All]" allUniqueName="[Schedule].[HD?].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Schedule].[SAP?]" caption="SAP?" attribute="1" defaultMemberUniqueName="[Schedule].[SAP?].[All]" allUniqueName="[Schedule].[SAP?].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Schedule].[Start Date Mismatch]" caption="Start Date Mismatch" attribute="1" defaultMemberUniqueName="[Schedule].[Start Date Mismatch].[All]" allUniqueName="[Schedule].[Start Date Mismatch].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Schedule].[Task Code]" caption="Task Code" attribute="1" defaultMemberUniqueName="[Schedule].[Task Code].[All]" allUniqueName="[Schedule].[Task Code].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Schedule].[Task Name]" caption="Task Name" attribute="1" defaultMemberUniqueName="[Schedule].[Task Name].[All]" allUniqueName="[Schedule].[Task Name].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Schedule].[Task Name Short]" caption="Task Name Short" attribute="1" defaultMemberUniqueName="[Schedule].[Task Name Short].[All]" allUniqueName="[Schedule].[Task Name Short].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Schedule].[Task Start Date]" caption="Task Start Date" attribute="1" defaultMemberUniqueName="[Schedule].[Task Start Date].[All]" allUniqueName="[Schedule].[Task Start Date].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0"/>
-    <cacheHierarchy uniqueName="[Cost Center Distinct].[COST_CENTER]" caption="COST_CENTER" attribute="1" defaultMemberUniqueName="[Cost Center Distinct].[COST_CENTER].[All]" allUniqueName="[Cost Center Distinct].[COST_CENTER].[All]" dimensionUniqueName="[Cost Center Distinct]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cost Center MPS].[CO_VERSION_ID]" caption="CO_VERSION_ID" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[CO_VERSION_ID].[All]" allUniqueName="[Cost Center MPS].[CO_VERSION_ID].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cost Center MPS].[COST_CENTER]" caption="COST_CENTER" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[COST_CENTER].[All]" allUniqueName="[Cost Center MPS].[COST_CENTER].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cost Center MPS].[DIRECT_MPS]" caption="DIRECT_MPS" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[DIRECT_MPS].[All]" allUniqueName="[Cost Center MPS].[DIRECT_MPS].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cost Center MPS].[EARNED_MPS]" caption="EARNED_MPS" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[EARNED_MPS].[All]" allUniqueName="[Cost Center MPS].[EARNED_MPS].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cost Center MPS].[INDIRECT_MPS]" caption="INDIRECT_MPS" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[INDIRECT_MPS].[All]" allUniqueName="[Cost Center MPS].[INDIRECT_MPS].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cost Center MPS].[OT_MPS]" caption="OT_MPS" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[OT_MPS].[All]" allUniqueName="[Cost Center MPS].[OT_MPS].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cost Center MPS].[WORKDAY_DATE]" caption="WORKDAY_DATE" attribute="1" defaultMemberUniqueName="[Cost Center MPS].[WORKDAY_DATE].[All]" allUniqueName="[Cost Center MPS].[WORKDAY_DATE].[All]" dimensionUniqueName="[Cost Center MPS]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Cost Centers].[COST_CENTER_KEY]" caption="COST_CENTER_KEY" attribute="1" defaultMemberUniqueName="[Cost Centers].[COST_CENTER_KEY].[All]" allUniqueName="[Cost Centers].[COST_CENTER_KEY].[All]" dimensionUniqueName="[Cost Centers]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Functions].[FUNCTION_GROUP_SORT]" caption="FUNCTION_GROUP_SORT" attribute="1" defaultMemberUniqueName="[Functions].[FUNCTION_GROUP_SORT].[All]" allUniqueName="[Functions].[FUNCTION_GROUP_SORT].[All]" dimensionUniqueName="[Functions]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[COST_CENTER_KEY]" caption="COST_CENTER_KEY" attribute="1" defaultMemberUniqueName="[HD Schedule].[COST_CENTER_KEY].[All]" allUniqueName="[HD Schedule].[COST_CENTER_KEY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HD_HRS_ACTUAL]" caption="DAILY_HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HD_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[DAILY_HD_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HD_HRS_EARNED]" caption="DAILY_HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HD_HRS_EARNED].[All]" allUniqueName="[HD Schedule].[DAILY_HD_HRS_EARNED].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HD_HRS_REMAINING]" caption="DAILY_HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HD_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[DAILY_HD_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HRS_ACTUAL]" caption="DAILY_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[DAILY_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HRS_CURR_EST]" caption="DAILY_HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HRS_CURR_EST].[All]" allUniqueName="[HD Schedule].[DAILY_HRS_CURR_EST].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HRS_REMAINING]" caption="DAILY_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[DAILY_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_HRS_TARGET]" caption="DAILY_HRS_TARGET" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_HRS_TARGET].[All]" allUniqueName="[HD Schedule].[DAILY_HRS_TARGET].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_SAP_HRS_ACTUAL]" caption="DAILY_SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_SAP_HRS_EARNED]" caption="DAILY_SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_SAP_HRS_EARNED].[All]" allUniqueName="[HD Schedule].[DAILY_SAP_HRS_EARNED].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_SAP_HRS_PLAN]" caption="DAILY_SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_SAP_HRS_PLAN].[All]" allUniqueName="[HD Schedule].[DAILY_SAP_HRS_PLAN].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[DAILY_SAP_HRS_REMAINING]" caption="DAILY_SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[DAILY_SAP_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[DAILY_SAP_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[Function Group]" caption="Function Group" attribute="1" defaultMemberUniqueName="[HD Schedule].[Function Group].[All]" allUniqueName="[HD Schedule].[Function Group].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[FUNCTION_CD]" caption="FUNCTION_CD" attribute="1" defaultMemberUniqueName="[HD Schedule].[FUNCTION_CD].[All]" allUniqueName="[HD Schedule].[FUNCTION_CD].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[FUNCTION_GROUP_SORT]" caption="FUNCTION_GROUP_SORT" attribute="1" defaultMemberUniqueName="[HD Schedule].[FUNCTION_GROUP_SORT].[All]" allUniqueName="[HD Schedule].[FUNCTION_GROUP_SORT].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[HD_FINISH_DATE]" caption="HD_FINISH_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_FINISH_DATE].[All]" allUniqueName="[HD Schedule].[HD_FINISH_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[HD_FLAG]" caption="HD_FLAG" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_FLAG].[All]" allUniqueName="[HD Schedule].[HD_FLAG].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[HD_HRS_ACTUAL]" caption="HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[HD_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[HD_HRS_EARNED]" caption="HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_HRS_EARNED].[All]" allUniqueName="[HD Schedule].[HD_HRS_EARNED].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[HD_HRS_REMAINING]" caption="HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[HD_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[HD_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[HRS_CURR_EST]" caption="HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[HD Schedule].[HRS_CURR_EST].[All]" allUniqueName="[HD Schedule].[HRS_CURR_EST].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[P6_EARLY_END_DATE]" caption="P6_EARLY_END_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_EARLY_END_DATE].[All]" allUniqueName="[HD Schedule].[P6_EARLY_END_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[P6_EARLY_START_DATE]" caption="P6_EARLY_START_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_EARLY_START_DATE].[All]" allUniqueName="[HD Schedule].[P6_EARLY_START_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[P6_END_DATE]" caption="P6_END_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_END_DATE].[All]" allUniqueName="[HD Schedule].[P6_END_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[P6_LATE_END_DATE]" caption="P6_LATE_END_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_LATE_END_DATE].[All]" allUniqueName="[HD Schedule].[P6_LATE_END_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[P6_LATE_START_DATE]" caption="P6_LATE_START_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_LATE_START_DATE].[All]" allUniqueName="[HD Schedule].[P6_LATE_START_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[P6_START_DATE]" caption="P6_START_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[P6_START_DATE].[All]" allUniqueName="[HD Schedule].[P6_START_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[PROD_GRP]" caption="PROD_GRP" attribute="1" defaultMemberUniqueName="[HD Schedule].[PROD_GRP].[All]" allUniqueName="[HD Schedule].[PROD_GRP].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[PRODUCT_CD_SHORT]" caption="PRODUCT_CD_SHORT" attribute="1" defaultMemberUniqueName="[HD Schedule].[PRODUCT_CD_SHORT].[All]" allUniqueName="[HD Schedule].[PRODUCT_CD_SHORT].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[PROJ_SHORT_NAME]" caption="PROJ_SHORT_NAME" attribute="1" defaultMemberUniqueName="[HD Schedule].[PROJ_SHORT_NAME].[All]" allUniqueName="[HD Schedule].[PROJ_SHORT_NAME].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[QTY_ACTUAL]" caption="QTY_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[QTY_ACTUAL].[All]" allUniqueName="[HD Schedule].[QTY_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[QTY_CURR_EST]" caption="QTY_CURR_EST" attribute="1" defaultMemberUniqueName="[HD Schedule].[QTY_CURR_EST].[All]" allUniqueName="[HD Schedule].[QTY_CURR_EST].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[QTY_ROLLUP_KEY]" caption="QTY_ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[HD Schedule].[QTY_ROLLUP_KEY].[All]" allUniqueName="[HD Schedule].[QTY_ROLLUP_KEY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[ROLLUP_KEY]" caption="ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[HD Schedule].[ROLLUP_KEY].[All]" allUniqueName="[HD Schedule].[ROLLUP_KEY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[SAP_FINISH_DATE]" caption="SAP_FINISH_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_FINISH_DATE].[All]" allUniqueName="[HD Schedule].[SAP_FINISH_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[SAP_FLAG]" caption="SAP_FLAG" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_FLAG].[All]" allUniqueName="[HD Schedule].[SAP_FLAG].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[SAP_HRS_ACTUAL]" caption="SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_HRS_ACTUAL].[All]" allUniqueName="[HD Schedule].[SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[SAP_HRS_EARNED]" caption="SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_HRS_EARNED].[All]" allUniqueName="[HD Schedule].[SAP_HRS_EARNED].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[SAP_HRS_PLAN]" caption="SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_HRS_PLAN].[All]" allUniqueName="[HD Schedule].[SAP_HRS_PLAN].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[SAP_HRS_REMAINING]" caption="SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_HRS_REMAINING].[All]" allUniqueName="[HD Schedule].[SAP_HRS_REMAINING].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[SAP_QTY]" caption="SAP_QTY" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_QTY].[All]" allUniqueName="[HD Schedule].[SAP_QTY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[SAP_QTY_COMPLETE]" caption="SAP_QTY_COMPLETE" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_QTY_COMPLETE].[All]" allUniqueName="[HD Schedule].[SAP_QTY_COMPLETE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[SAP_START_DATE]" caption="SAP_START_DATE" attribute="1" defaultMemberUniqueName="[HD Schedule].[SAP_START_DATE].[All]" allUniqueName="[HD Schedule].[SAP_START_DATE].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[TARGET_WORK_QTY]" caption="TARGET_WORK_QTY" attribute="1" defaultMemberUniqueName="[HD Schedule].[TARGET_WORK_QTY].[All]" allUniqueName="[HD Schedule].[TARGET_WORK_QTY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[WORK_DAY]" caption="WORK_DAY" attribute="1" defaultMemberUniqueName="[HD Schedule].[WORK_DAY].[All]" allUniqueName="[HD Schedule].[WORK_DAY].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[HD Schedule].[WORK_DAY_COUNT]" caption="WORK_DAY_COUNT" attribute="1" defaultMemberUniqueName="[HD Schedule].[WORK_DAY_COUNT].[All]" allUniqueName="[HD Schedule].[WORK_DAY_COUNT].[All]" dimensionUniqueName="[HD Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[LAST_UPDATED]" caption="LAST_UPDATED" attribute="1" defaultMemberUniqueName="[Job Shipments].[LAST_UPDATED].[All]" allUniqueName="[Job Shipments].[LAST_UPDATED].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[PROJ_ID]" caption="PROJ_ID" attribute="1" defaultMemberUniqueName="[Job Shipments].[PROJ_ID].[All]" allUniqueName="[Job Shipments].[PROJ_ID].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Job Shipments].[SHIP_DATES_DIFF]" caption="SHIP_DATES_DIFF" attribute="1" defaultMemberUniqueName="[Job Shipments].[SHIP_DATES_DIFF].[All]" allUniqueName="[Job Shipments].[SHIP_DATES_DIFF].[All]" dimensionUniqueName="[Job Shipments]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[BAY]" caption="BAY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[BAY].[All]" allUniqueName="[Late End Schedule].[BAY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[COST_CENTER]" caption="COST_CENTER" attribute="1" defaultMemberUniqueName="[Late End Schedule].[COST_CENTER].[All]" allUniqueName="[Late End Schedule].[COST_CENTER].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[COST_CENTER_DESC]" caption="COST_CENTER_DESC" attribute="1" defaultMemberUniqueName="[Late End Schedule].[COST_CENTER_DESC].[All]" allUniqueName="[Late End Schedule].[COST_CENTER_DESC].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[COST_CENTER_KEY]" caption="COST_CENTER_KEY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[COST_CENTER_KEY].[All]" allUniqueName="[Late End Schedule].[COST_CENTER_KEY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HD_HRS_ACTUAL]" caption="DAILY_HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HD_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[DAILY_HD_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HD_HRS_EARNED]" caption="DAILY_HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HD_HRS_EARNED].[All]" allUniqueName="[Late End Schedule].[DAILY_HD_HRS_EARNED].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HD_HRS_REMAINING]" caption="DAILY_HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HD_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[DAILY_HD_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HRS_ACTUAL]" caption="DAILY_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[DAILY_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HRS_CURR_EST]" caption="DAILY_HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HRS_CURR_EST].[All]" allUniqueName="[Late End Schedule].[DAILY_HRS_CURR_EST].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HRS_REMAINING]" caption="DAILY_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[DAILY_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_HRS_TARGET]" caption="DAILY_HRS_TARGET" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_HRS_TARGET].[All]" allUniqueName="[Late End Schedule].[DAILY_HRS_TARGET].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_SAP_HRS_ACTUAL]" caption="DAILY_SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_SAP_HRS_EARNED]" caption="DAILY_SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_SAP_HRS_EARNED].[All]" allUniqueName="[Late End Schedule].[DAILY_SAP_HRS_EARNED].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_SAP_HRS_PLAN]" caption="DAILY_SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_SAP_HRS_PLAN].[All]" allUniqueName="[Late End Schedule].[DAILY_SAP_HRS_PLAN].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[DAILY_SAP_HRS_REMAINING]" caption="DAILY_SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[DAILY_SAP_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[DAILY_SAP_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[FINISH_DATE_MISMATCH]" caption="FINISH_DATE_MISMATCH" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FINISH_DATE_MISMATCH].[All]" allUniqueName="[Late End Schedule].[FINISH_DATE_MISMATCH].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[FUNCTION_CD]" caption="FUNCTION_CD" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FUNCTION_CD].[All]" allUniqueName="[Late End Schedule].[FUNCTION_CD].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[FUNCTION_DESC]" caption="FUNCTION_DESC" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FUNCTION_DESC].[All]" allUniqueName="[Late End Schedule].[FUNCTION_DESC].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[FUNCTION_GROUP]" caption="FUNCTION_GROUP" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FUNCTION_GROUP].[All]" allUniqueName="[Late End Schedule].[FUNCTION_GROUP].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[FUNCTION_GROUP_SORT]" caption="FUNCTION_GROUP_SORT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[FUNCTION_GROUP_SORT].[All]" allUniqueName="[Late End Schedule].[FUNCTION_GROUP_SORT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[HD_FINISH_DATE]" caption="HD_FINISH_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_FINISH_DATE].[All]" allUniqueName="[Late End Schedule].[HD_FINISH_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[HD_HRS_ACTUAL]" caption="HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[HD_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[HD_HRS_EARNED]" caption="HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_HRS_EARNED].[All]" allUniqueName="[Late End Schedule].[HD_HRS_EARNED].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[HD_HRS_REMAINING]" caption="HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[HD_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[HD_RESOURCE]" caption="HD_RESOURCE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_RESOURCE].[All]" allUniqueName="[Late End Schedule].[HD_RESOURCE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[HD_START_DATE]" caption="HD_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HD_START_DATE].[All]" allUniqueName="[Late End Schedule].[HD_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[HEIGHT]" caption="HEIGHT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HEIGHT].[All]" allUniqueName="[Late End Schedule].[HEIGHT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[HRS_CURR_EST]" caption="HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[Late End Schedule].[HRS_CURR_EST].[All]" allUniqueName="[Late End Schedule].[HRS_CURR_EST].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[LENGTH]" caption="LENGTH" attribute="1" defaultMemberUniqueName="[Late End Schedule].[LENGTH].[All]" allUniqueName="[Late End Schedule].[LENGTH].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[P6_EARLY_END_DATE]" caption="P6_EARLY_END_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_EARLY_END_DATE].[All]" allUniqueName="[Late End Schedule].[P6_EARLY_END_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[P6_EARLY_START_DATE]" caption="P6_EARLY_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_EARLY_START_DATE].[All]" allUniqueName="[Late End Schedule].[P6_EARLY_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[P6_END_DATE]" caption="P6_END_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_END_DATE].[All]" allUniqueName="[Late End Schedule].[P6_END_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[P6_LATE_END_DATE]" caption="P6_LATE_END_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_LATE_END_DATE].[All]" allUniqueName="[Late End Schedule].[P6_LATE_END_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[P6_LATE_START_DATE]" caption="P6_LATE_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_LATE_START_DATE].[All]" allUniqueName="[Late End Schedule].[P6_LATE_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[P6_SHIP_DATE]" caption="P6_SHIP_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_SHIP_DATE].[All]" allUniqueName="[Late End Schedule].[P6_SHIP_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[P6_SHIP_MONTH_YEAR]" caption="P6_SHIP_MONTH_YEAR" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_SHIP_MONTH_YEAR].[All]" allUniqueName="[Late End Schedule].[P6_SHIP_MONTH_YEAR].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[P6_SHIP_YEAR_MONTH]" caption="P6_SHIP_YEAR_MONTH" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_SHIP_YEAR_MONTH].[All]" allUniqueName="[Late End Schedule].[P6_SHIP_YEAR_MONTH].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[P6_START_DATE]" caption="P6_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[P6_START_DATE].[All]" allUniqueName="[Late End Schedule].[P6_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[PLANT]" caption="PLANT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PLANT].[All]" allUniqueName="[Late End Schedule].[PLANT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[PLANT_ID]" caption="PLANT_ID" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PLANT_ID].[All]" allUniqueName="[Late End Schedule].[PLANT_ID].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[PROD_GRP]" caption="PROD_GRP" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PROD_GRP].[All]" allUniqueName="[Late End Schedule].[PROD_GRP].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[PROD_GRP_DESC]" caption="PROD_GRP_DESC" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PROD_GRP_DESC].[All]" allUniqueName="[Late End Schedule].[PROD_GRP_DESC].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[PRODUCT_CD]" caption="PRODUCT_CD" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PRODUCT_CD].[All]" allUniqueName="[Late End Schedule].[PRODUCT_CD].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[PRODUCT_CD_SHORT]" caption="PRODUCT_CD_SHORT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PRODUCT_CD_SHORT].[All]" allUniqueName="[Late End Schedule].[PRODUCT_CD_SHORT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[PROJ_ID]" caption="PROJ_ID" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PROJ_ID].[All]" allUniqueName="[Late End Schedule].[PROJ_ID].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[PROJ_SHORT_NAME]" caption="PROJ_SHORT_NAME" attribute="1" defaultMemberUniqueName="[Late End Schedule].[PROJ_SHORT_NAME].[All]" allUniqueName="[Late End Schedule].[PROJ_SHORT_NAME].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[QTY_ACTUAL]" caption="QTY_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[QTY_ACTUAL].[All]" allUniqueName="[Late End Schedule].[QTY_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[QTY_CURR_EST]" caption="QTY_CURR_EST" attribute="1" defaultMemberUniqueName="[Late End Schedule].[QTY_CURR_EST].[All]" allUniqueName="[Late End Schedule].[QTY_CURR_EST].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[QTY_ROLLUP_KEY]" caption="QTY_ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[QTY_ROLLUP_KEY].[All]" allUniqueName="[Late End Schedule].[QTY_ROLLUP_KEY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[ROLLUP_KEY]" caption="ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[ROLLUP_KEY].[All]" allUniqueName="[Late End Schedule].[ROLLUP_KEY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_FINISH_DATE]" caption="SAP_FINISH_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_FINISH_DATE].[All]" allUniqueName="[Late End Schedule].[SAP_FINISH_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_HRS_ACTUAL]" caption="SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_HRS_ACTUAL].[All]" allUniqueName="[Late End Schedule].[SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_HRS_EARNED]" caption="SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_HRS_EARNED].[All]" allUniqueName="[Late End Schedule].[SAP_HRS_EARNED].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_HRS_PLAN]" caption="SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_HRS_PLAN].[All]" allUniqueName="[Late End Schedule].[SAP_HRS_PLAN].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_HRS_REMAINING]" caption="SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_HRS_REMAINING].[All]" allUniqueName="[Late End Schedule].[SAP_HRS_REMAINING].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_QTY]" caption="SAP_QTY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_QTY].[All]" allUniqueName="[Late End Schedule].[SAP_QTY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_QTY_COMPLETE]" caption="SAP_QTY_COMPLETE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_QTY_COMPLETE].[All]" allUniqueName="[Late End Schedule].[SAP_QTY_COMPLETE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[SAP_START_DATE]" caption="SAP_START_DATE" attribute="1" defaultMemberUniqueName="[Late End Schedule].[SAP_START_DATE].[All]" allUniqueName="[Late End Schedule].[SAP_START_DATE].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[START_DATE_MISMATCH]" caption="START_DATE_MISMATCH" attribute="1" defaultMemberUniqueName="[Late End Schedule].[START_DATE_MISMATCH].[All]" allUniqueName="[Late End Schedule].[START_DATE_MISMATCH].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[TARGET_WORK_QTY]" caption="TARGET_WORK_QTY" attribute="1" defaultMemberUniqueName="[Late End Schedule].[TARGET_WORK_QTY].[All]" allUniqueName="[Late End Schedule].[TARGET_WORK_QTY].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[WORK_CENTER]" caption="WORK_CENTER" attribute="1" defaultMemberUniqueName="[Late End Schedule].[WORK_CENTER].[All]" allUniqueName="[Late End Schedule].[WORK_CENTER].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[WORK_CENTER_DESC]" caption="WORK_CENTER_DESC" attribute="1" defaultMemberUniqueName="[Late End Schedule].[WORK_CENTER_DESC].[All]" allUniqueName="[Late End Schedule].[WORK_CENTER_DESC].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Late End Schedule].[WORK_DAY_COUNT]" caption="WORK_DAY_COUNT" attribute="1" defaultMemberUniqueName="[Late End Schedule].[WORK_DAY_COUNT].[All]" allUniqueName="[Late End Schedule].[WORK_DAY_COUNT].[All]" dimensionUniqueName="[Late End Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Measures].[COLUMN1]" caption="COLUMN1" attribute="1" defaultMemberUniqueName="[Milestone Measures].[COLUMN1].[All]" allUniqueName="[Milestone Measures].[COLUMN1].[All]" dimensionUniqueName="[Milestone Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Measures].[COLUMN2]" caption="COLUMN2" attribute="1" defaultMemberUniqueName="[Milestone Measures].[COLUMN2].[All]" allUniqueName="[Milestone Measures].[COLUMN2].[All]" dimensionUniqueName="[Milestone Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Measures].[COLUMN3]" caption="COLUMN3" attribute="1" defaultMemberUniqueName="[Milestone Measures].[COLUMN3].[All]" allUniqueName="[Milestone Measures].[COLUMN3].[All]" dimensionUniqueName="[Milestone Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[ACTUAL_DATE]" caption="ACTUAL_DATE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[ACTUAL_DATE].[All]" allUniqueName="[Milestone Schedule].[ACTUAL_DATE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[DAYS_OUT]" caption="DAYS_OUT" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[DAYS_OUT].[All]" allUniqueName="[Milestone Schedule].[DAYS_OUT].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[DUE_DATE]" caption="DUE_DATE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[DUE_DATE].[All]" allUniqueName="[Milestone Schedule].[DUE_DATE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[MATL_MISSING]" caption="MATL_MISSING" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[MATL_MISSING].[All]" allUniqueName="[Milestone Schedule].[MATL_MISSING].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[MILESTONE_GROUP_SORT]" caption="MILESTONE_GROUP_SORT" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[MILESTONE_GROUP_SORT].[All]" allUniqueName="[Milestone Schedule].[MILESTONE_GROUP_SORT].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[MILESTONE_SORT]" caption="MILESTONE_SORT" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[MILESTONE_SORT].[All]" allUniqueName="[Milestone Schedule].[MILESTONE_SORT].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[MILESTONE_STATUS_VALUE]" caption="MILESTONE_STATUS_VALUE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[MILESTONE_STATUS_VALUE].[All]" allUniqueName="[Milestone Schedule].[MILESTONE_STATUS_VALUE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[ORDER_QTY]" caption="ORDER_QTY" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[ORDER_QTY].[All]" allUniqueName="[Milestone Schedule].[ORDER_QTY].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[P6_PROJ_SHORT_NAME]" caption="P6_PROJ_SHORT_NAME" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[P6_PROJ_SHORT_NAME].[All]" allUniqueName="[Milestone Schedule].[P6_PROJ_SHORT_NAME].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[PLOT_DUE_DATE]" caption="PLOT_DUE_DATE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[PLOT_DUE_DATE].[All]" allUniqueName="[Milestone Schedule].[PLOT_DUE_DATE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[QTY_RECVD]" caption="QTY_RECVD" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[QTY_RECVD].[All]" allUniqueName="[Milestone Schedule].[QTY_RECVD].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Milestone Schedule].[REFERENCE_DATE]" caption="REFERENCE_DATE" attribute="1" defaultMemberUniqueName="[Milestone Schedule].[REFERENCE_DATE].[All]" allUniqueName="[Milestone Schedule].[REFERENCE_DATE].[All]" dimensionUniqueName="[Milestone Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Public Schedule Measures].[COLUMN1]" caption="COLUMN1" attribute="1" defaultMemberUniqueName="[Public Schedule Measures].[COLUMN1].[All]" allUniqueName="[Public Schedule Measures].[COLUMN1].[All]" dimensionUniqueName="[Public Schedule Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Public Schedule Measures].[COLUMN2]" caption="COLUMN2" attribute="1" defaultMemberUniqueName="[Public Schedule Measures].[COLUMN2].[All]" allUniqueName="[Public Schedule Measures].[COLUMN2].[All]" dimensionUniqueName="[Public Schedule Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Public Schedule Measures].[COLUMN3]" caption="COLUMN3" attribute="1" defaultMemberUniqueName="[Public Schedule Measures].[COLUMN3].[All]" allUniqueName="[Public Schedule Measures].[COLUMN3].[All]" dimensionUniqueName="[Public Schedule Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[BAY]" caption="BAY" attribute="1" defaultMemberUniqueName="[Schedule].[BAY].[All]" allUniqueName="[Schedule].[BAY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[COST_CENTER]" caption="COST_CENTER" attribute="1" defaultMemberUniqueName="[Schedule].[COST_CENTER].[All]" allUniqueName="[Schedule].[COST_CENTER].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[COST_CENTER_DESC]" caption="COST_CENTER_DESC" attribute="1" defaultMemberUniqueName="[Schedule].[COST_CENTER_DESC].[All]" allUniqueName="[Schedule].[COST_CENTER_DESC].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[COST_CENTER_KEY]" caption="COST_CENTER_KEY" attribute="1" defaultMemberUniqueName="[Schedule].[COST_CENTER_KEY].[All]" allUniqueName="[Schedule].[COST_CENTER_KEY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_HD_HRS_ACTUAL]" caption="DAILY_HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HD_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[DAILY_HD_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_HD_HRS_EARNED]" caption="DAILY_HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HD_HRS_EARNED].[All]" allUniqueName="[Schedule].[DAILY_HD_HRS_EARNED].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_HD_HRS_REMAINING]" caption="DAILY_HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HD_HRS_REMAINING].[All]" allUniqueName="[Schedule].[DAILY_HD_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_HRS_ACTUAL]" caption="DAILY_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[DAILY_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_HRS_CURR_EST]" caption="DAILY_HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HRS_CURR_EST].[All]" allUniqueName="[Schedule].[DAILY_HRS_CURR_EST].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_HRS_REMAINING]" caption="DAILY_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HRS_REMAINING].[All]" allUniqueName="[Schedule].[DAILY_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_HRS_TARGET]" caption="DAILY_HRS_TARGET" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_HRS_TARGET].[All]" allUniqueName="[Schedule].[DAILY_HRS_TARGET].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_SAP_HRS_ACTUAL]" caption="DAILY_SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[DAILY_SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_SAP_HRS_EARNED]" caption="DAILY_SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_SAP_HRS_EARNED].[All]" allUniqueName="[Schedule].[DAILY_SAP_HRS_EARNED].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_SAP_HRS_PLAN]" caption="DAILY_SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_SAP_HRS_PLAN].[All]" allUniqueName="[Schedule].[DAILY_SAP_HRS_PLAN].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[DAILY_SAP_HRS_REMAINING]" caption="DAILY_SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[DAILY_SAP_HRS_REMAINING].[All]" allUniqueName="[Schedule].[DAILY_SAP_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[Function Group]" caption="Function Group" attribute="1" defaultMemberUniqueName="[Schedule].[Function Group].[All]" allUniqueName="[Schedule].[Function Group].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[FUNCTION_CD]" caption="FUNCTION_CD" attribute="1" defaultMemberUniqueName="[Schedule].[FUNCTION_CD].[All]" allUniqueName="[Schedule].[FUNCTION_CD].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[FUNCTION_DESC]" caption="FUNCTION_DESC" attribute="1" defaultMemberUniqueName="[Schedule].[FUNCTION_DESC].[All]" allUniqueName="[Schedule].[FUNCTION_DESC].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[FUNCTION_GROUP_SORT]" caption="FUNCTION_GROUP_SORT" attribute="1" defaultMemberUniqueName="[Schedule].[FUNCTION_GROUP_SORT].[All]" allUniqueName="[Schedule].[FUNCTION_GROUP_SORT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[HD_FINISH_DATE]" caption="HD_FINISH_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[HD_FINISH_DATE].[All]" allUniqueName="[Schedule].[HD_FINISH_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[HD_HRS_ACTUAL]" caption="HD_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[HD_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[HD_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[HD_HRS_EARNED]" caption="HD_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Schedule].[HD_HRS_EARNED].[All]" allUniqueName="[Schedule].[HD_HRS_EARNED].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[HD_HRS_REMAINING]" caption="HD_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[HD_HRS_REMAINING].[All]" allUniqueName="[Schedule].[HD_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[HD_RESOURCE]" caption="HD_RESOURCE" attribute="1" defaultMemberUniqueName="[Schedule].[HD_RESOURCE].[All]" allUniqueName="[Schedule].[HD_RESOURCE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[HD_START_DATE]" caption="HD_START_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[HD_START_DATE].[All]" allUniqueName="[Schedule].[HD_START_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[HEIGHT]" caption="HEIGHT" attribute="1" defaultMemberUniqueName="[Schedule].[HEIGHT].[All]" allUniqueName="[Schedule].[HEIGHT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[HRS_CURR_EST]" caption="HRS_CURR_EST" attribute="1" defaultMemberUniqueName="[Schedule].[HRS_CURR_EST].[All]" allUniqueName="[Schedule].[HRS_CURR_EST].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[LENGTH]" caption="LENGTH" attribute="1" defaultMemberUniqueName="[Schedule].[LENGTH].[All]" allUniqueName="[Schedule].[LENGTH].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[P6_EARLY_END_DATE]" caption="P6_EARLY_END_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_EARLY_END_DATE].[All]" allUniqueName="[Schedule].[P6_EARLY_END_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[P6_END_DATE]" caption="P6_END_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_END_DATE].[All]" allUniqueName="[Schedule].[P6_END_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[P6_LATE_END_DATE]" caption="P6_LATE_END_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_LATE_END_DATE].[All]" allUniqueName="[Schedule].[P6_LATE_END_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[P6_LATE_START_DATE]" caption="P6_LATE_START_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_LATE_START_DATE].[All]" allUniqueName="[Schedule].[P6_LATE_START_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[P6_SHIP_DATE]" caption="P6_SHIP_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_SHIP_DATE].[All]" allUniqueName="[Schedule].[P6_SHIP_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[P6_SHIP_MONTH_YEAR]" caption="P6_SHIP_MONTH_YEAR" attribute="1" defaultMemberUniqueName="[Schedule].[P6_SHIP_MONTH_YEAR].[All]" allUniqueName="[Schedule].[P6_SHIP_MONTH_YEAR].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[P6_SHIP_YEAR_MONTH]" caption="P6_SHIP_YEAR_MONTH" attribute="1" defaultMemberUniqueName="[Schedule].[P6_SHIP_YEAR_MONTH].[All]" allUniqueName="[Schedule].[P6_SHIP_YEAR_MONTH].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[P6_START_DATE]" caption="P6_START_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[P6_START_DATE].[All]" allUniqueName="[Schedule].[P6_START_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[PLANT]" caption="PLANT" attribute="1" defaultMemberUniqueName="[Schedule].[PLANT].[All]" allUniqueName="[Schedule].[PLANT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[PLANT_ID]" caption="PLANT_ID" attribute="1" defaultMemberUniqueName="[Schedule].[PLANT_ID].[All]" allUniqueName="[Schedule].[PLANT_ID].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[PROD_GRP]" caption="PROD_GRP" attribute="1" defaultMemberUniqueName="[Schedule].[PROD_GRP].[All]" allUniqueName="[Schedule].[PROD_GRP].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[PROD_GRP_DESC]" caption="PROD_GRP_DESC" attribute="1" defaultMemberUniqueName="[Schedule].[PROD_GRP_DESC].[All]" allUniqueName="[Schedule].[PROD_GRP_DESC].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[PRODUCT_CD]" caption="PRODUCT_CD" attribute="1" defaultMemberUniqueName="[Schedule].[PRODUCT_CD].[All]" allUniqueName="[Schedule].[PRODUCT_CD].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[PRODUCT_CD_SHORT]" caption="PRODUCT_CD_SHORT" attribute="1" defaultMemberUniqueName="[Schedule].[PRODUCT_CD_SHORT].[All]" allUniqueName="[Schedule].[PRODUCT_CD_SHORT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[PROJ_ID]" caption="PROJ_ID" attribute="1" defaultMemberUniqueName="[Schedule].[PROJ_ID].[All]" allUniqueName="[Schedule].[PROJ_ID].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[PROJ_SHORT_NAME]" caption="PROJ_SHORT_NAME" attribute="1" defaultMemberUniqueName="[Schedule].[PROJ_SHORT_NAME].[All]" allUniqueName="[Schedule].[PROJ_SHORT_NAME].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[QTY_ACTUAL]" caption="QTY_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[QTY_ACTUAL].[All]" allUniqueName="[Schedule].[QTY_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[QTY_CURR_EST]" caption="QTY_CURR_EST" attribute="1" defaultMemberUniqueName="[Schedule].[QTY_CURR_EST].[All]" allUniqueName="[Schedule].[QTY_CURR_EST].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[QTY_ROLLUP_KEY]" caption="QTY_ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[Schedule].[QTY_ROLLUP_KEY].[All]" allUniqueName="[Schedule].[QTY_ROLLUP_KEY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[ROLLUP_KEY]" caption="ROLLUP_KEY" attribute="1" defaultMemberUniqueName="[Schedule].[ROLLUP_KEY].[All]" allUniqueName="[Schedule].[ROLLUP_KEY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[SAP_FINISH_DATE]" caption="SAP_FINISH_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_FINISH_DATE].[All]" allUniqueName="[Schedule].[SAP_FINISH_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[SAP_HRS_ACTUAL]" caption="SAP_HRS_ACTUAL" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_HRS_ACTUAL].[All]" allUniqueName="[Schedule].[SAP_HRS_ACTUAL].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[SAP_HRS_EARNED]" caption="SAP_HRS_EARNED" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_HRS_EARNED].[All]" allUniqueName="[Schedule].[SAP_HRS_EARNED].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[SAP_HRS_PLAN]" caption="SAP_HRS_PLAN" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_HRS_PLAN].[All]" allUniqueName="[Schedule].[SAP_HRS_PLAN].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[SAP_HRS_REMAINING]" caption="SAP_HRS_REMAINING" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_HRS_REMAINING].[All]" allUniqueName="[Schedule].[SAP_HRS_REMAINING].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[SAP_QTY]" caption="SAP_QTY" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_QTY].[All]" allUniqueName="[Schedule].[SAP_QTY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[SAP_QTY_COMPLETE]" caption="SAP_QTY_COMPLETE" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_QTY_COMPLETE].[All]" allUniqueName="[Schedule].[SAP_QTY_COMPLETE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[SAP_START_DATE]" caption="SAP_START_DATE" attribute="1" defaultMemberUniqueName="[Schedule].[SAP_START_DATE].[All]" allUniqueName="[Schedule].[SAP_START_DATE].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[TARGET_WORK_QTY]" caption="TARGET_WORK_QTY" attribute="1" defaultMemberUniqueName="[Schedule].[TARGET_WORK_QTY].[All]" allUniqueName="[Schedule].[TARGET_WORK_QTY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[WORK_CENTER]" caption="WORK_CENTER" attribute="1" defaultMemberUniqueName="[Schedule].[WORK_CENTER].[All]" allUniqueName="[Schedule].[WORK_CENTER].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[WORK_CENTER_DESC]" caption="WORK_CENTER_DESC" attribute="1" defaultMemberUniqueName="[Schedule].[WORK_CENTER_DESC].[All]" allUniqueName="[Schedule].[WORK_CENTER_DESC].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[WORK_DAY]" caption="WORK_DAY" attribute="1" defaultMemberUniqueName="[Schedule].[WORK_DAY].[All]" allUniqueName="[Schedule].[WORK_DAY].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Schedule].[WORK_DAY_COUNT]" caption="WORK_DAY_COUNT" attribute="1" defaultMemberUniqueName="[Schedule].[WORK_DAY_COUNT].[All]" allUniqueName="[Schedule].[WORK_DAY_COUNT].[All]" dimensionUniqueName="[Schedule]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Scheduling Measures].[COLUMN1]" caption="COLUMN1" attribute="1" defaultMemberUniqueName="[Scheduling Measures].[COLUMN1].[All]" allUniqueName="[Scheduling Measures].[COLUMN1].[All]" dimensionUniqueName="[Scheduling Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Scheduling Measures].[COLUMN2]" caption="COLUMN2" attribute="1" defaultMemberUniqueName="[Scheduling Measures].[COLUMN2].[All]" allUniqueName="[Scheduling Measures].[COLUMN2].[All]" dimensionUniqueName="[Scheduling Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Scheduling Measures].[COLUMN3]" caption="COLUMN3" attribute="1" defaultMemberUniqueName="[Scheduling Measures].[COLUMN3].[All]" allUniqueName="[Scheduling Measures].[COLUMN3].[All]" dimensionUniqueName="[Scheduling Measures]" displayFolder="" count="0" unbalanced="0" hidden="1"/>
-    <cacheHierarchy uniqueName="[Measures].[Milestone Days Out]" caption="Milestone Days Out" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Matl Order Qty]" caption="Matl Order Qty" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Matl Recvd Qty]" caption="Matl Recvd Qty" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Matl Missing Qty]" caption="Matl Missing Qty" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Milestone Due Date]" caption="Milestone Due Date" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Milestone Status Value]" caption="Milestone Status Value" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Milestone Days Overdue]" caption="Milestone Days Overdue" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Milestone Count]" caption="Milestone Count" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Completed Milestones]" caption="Completed Milestones" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Incomplete Milestones]" caption="Incomplete Milestones" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Milestone Group Status]" caption="Milestone Group Status" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Milestone Column Value 2 3]" caption="Milestone Column Value 2 3" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Milestone Column Value 1 4]" caption="Milestone Column Value 1 4" measure="1" displayFolder="" measureGroup="Milestone Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[P6 Remaining Hours]" caption="P6 Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[P6 Scheduled Remaining Hours]" caption="P6 Scheduled Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD Remaining Hours]" caption="HD Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD Scheduled Remaining Hours]" caption="HD Scheduled Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD Qty]" caption="HD Qty" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD Start Date]" caption="HD Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD End Date]" caption="HD End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Start Date]" caption="SAP Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP End Date]" caption="SAP End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Qty]" caption="SAP Qty" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Qty Complete]" caption="SAP Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Qty Remaining]" caption="SAP Qty Remaining" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Qty % Complete]" caption="SAP Qty % Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Plan Hours]" caption="SAP Plan Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Actual Hours]" caption="SAP Actual Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Earned Hours]" caption="SAP Earned Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Remaining Hours]" caption="SAP Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[SAP Scheduled Remaining Hours]" caption="SAP Scheduled Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[P6 Target Hours]" caption="P6 Target Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Remaining Hours Adjusted]" caption="Remaining Hours Adjusted" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD Earned Hours]" caption="HD Earned Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD Plan Hours]" caption="HD Plan Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD Qty Complete]" caption="HD Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD Qty Remaining]" caption="HD Qty Remaining" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[HD Qty % Complete]" caption="HD Qty % Complete" measure="1" displayFolder="Quantities" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Data Last Updated]" caption="Data Last Updated" measure="1" displayFolder="" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Ship Date Status Indicator]" caption="Ship Date Status Indicator" measure="1" displayFolder="Indicators" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Ship Date]" caption="Ship Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Earned MPS (004)]" caption="Earned MPS (004)" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Active Job Remaining Hours]" caption="Active Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Planned Job Remaining Hours]" caption="Planned Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Active Job Start Date]" caption="Active Job Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Planned Job Start Date]" caption="Planned Job Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Job Status Indicator]" caption="Job Status Indicator" measure="1" displayFolder="Indicators" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[What-If Job Remaining Hours]" caption="What-If Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Inactive Job Remaining Hours]" caption="Inactive Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[P6 Girder Start Date]" caption="P6 Girder Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[P6 Early Start Date]" caption="P6 Early Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[P6 Early End Date]" caption="P6 Early End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Fab Start Date]" caption="Fab Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Fab End Date]" caption="Fab End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Yard Start Date]" caption="Yard Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Yard End Date]" caption="Yard End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Coatings Start Date]" caption="Coatings Start Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Coatings End Date]" caption="Coatings End Date" measure="1" displayFolder="Dates" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[P6 Late Remaining Hours]" caption="P6 Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Active Job Late Remaining Hours]" caption="Active Job Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Planned Job Late Remaining Hours]" caption="Planned Job Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[What-If Job Late Remaining Hours]" caption="What-If Job Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Inactive Job Late Remaining Hours]" caption="Inactive Job Late Remaining Hours" measure="1" displayFolder="Late End Schedule" measureGroup="Scheduling Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Remaining Hours]" caption="Public Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Active Job Remaining Hours]" caption="Public Active Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Planned Job Remaining Hours]" caption="Public Planned Job Remaining Hours" measure="1" displayFolder="Hours" measureGroup="Public Schedule Measures" count="0"/>
-    <cacheHierarchy uniqueName="[Measures].[Public Start Date]" caption="Public Start Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Public End Date]" caption="Public End Date" measure="1" displayFolder="Dates" measureGroup="Public Schedule Measures" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Public HD Qty]" caption="Public HD Qty" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
     <cacheHierarchy uniqueName="[Measures].[Public HD Qty Complete]" caption="Public HD Qty Complete" measure="1" displayFolder="Quantities" measureGroup="Public Schedule Measures" count="0"/>
@@ -3500,7 +3506,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0000-000000000000}" name="PivotTable1" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:C200" firstHeaderRow="0" firstDataRow="1" firstDataCol="1"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" allDrilled="1" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -4763,7 +4769,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0100-000000000000}" name="PivotTable1" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:B201" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="2">
     <pivotField axis="axisRow" allDrilled="1" outline="0" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -6197,7 +6203,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="Products" cacheId="6" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0200-000000000000}" name="Products" cacheId="15" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:C205" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="3">
     <pivotField axis="axisRow" allDrilled="1" outline="0" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -7640,7 +7646,7 @@
 </file>
 
 <file path=xl/pivotTables/pivotTable4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="Bays" cacheId="9" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
+<pivotTableDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" xr:uid="{00000000-0007-0000-0300-000000000000}" name="Bays" cacheId="12" applyNumberFormats="0" applyBorderFormats="0" applyFontFormats="0" applyPatternFormats="0" applyAlignmentFormats="0" applyWidthHeightFormats="1" dataCaption="Values" updatedVersion="6" minRefreshableVersion="3" useAutoFormatting="1" subtotalHiddenItems="1" rowGrandTotals="0" colGrandTotals="0" itemPrintTitles="1" createdVersion="6" indent="0" outline="1" outlineData="1" multipleFieldFilters="0" fieldListSortAscending="1">
   <location ref="A1:C361" firstHeaderRow="1" firstDataRow="1" firstDataCol="2"/>
   <pivotFields count="4">
     <pivotField axis="axisRow" allDrilled="1" outline="0" subtotalTop="0" showAll="0" sortType="ascending" defaultSubtotal="0" defaultAttributeDrillState="1">
@@ -9880,7 +9886,9 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:C1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -12035,7 +12043,9 @@
   <sheetPr codeName="Sheet2"/>
   <dimension ref="A1:B201"/>
   <sheetViews>
-    <sheetView workbookViewId="0"/>
+    <sheetView workbookViewId="0">
+      <selection sqref="A1:B1"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <cols>
@@ -13740,7 +13750,7 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
+    <sheetView tabSelected="1" workbookViewId="0">
       <selection activeCell="G12" sqref="G12"/>
     </sheetView>
   </sheetViews>
@@ -16677,7 +16687,7 @@
         <v>215</v>
       </c>
       <c r="C57" s="3">
-        <v>43980</v>
+        <v>44193</v>
       </c>
     </row>
     <row r="58" spans="1:3" x14ac:dyDescent="0.25">
@@ -16721,7 +16731,7 @@
         <v>215</v>
       </c>
       <c r="C61" s="3">
-        <v>43980</v>
+        <v>44071</v>
       </c>
     </row>
     <row r="62" spans="1:3" x14ac:dyDescent="0.25">
@@ -16743,7 +16753,7 @@
         <v>215</v>
       </c>
       <c r="C63" s="3">
-        <v>43980</v>
+        <v>44188</v>
       </c>
     </row>
     <row r="64" spans="1:3" x14ac:dyDescent="0.25">
@@ -20030,12 +20040,15 @@
 </file>
 
 <file path=customXml/item1.xml><?xml version="1.0" encoding="utf-8"?>
-<?mso-contentType ?>
-<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
-  <Display>DocumentLibraryForm</Display>
-  <Edit>DocumentLibraryForm</Edit>
-  <New>DocumentLibraryForm</New>
-</FormTemplates>
+<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
+  <documentManagement>
+    <MigrationWizIdPermissions xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
+    <MigrationWizIdPermissionLevels xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
+    <MigrationWizIdDocumentLibraryPermissions xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
+    <MigrationWizIdSecurityGroups xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
+    <MigrationWizId xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
+  </documentManagement>
+</p:properties>
 </file>
 
 <file path=customXml/item2.xml><?xml version="1.0" encoding="utf-8"?>
@@ -20292,21 +20305,27 @@
 </file>
 
 <file path=customXml/item3.xml><?xml version="1.0" encoding="utf-8"?>
-<p:properties xmlns:p="http://schemas.microsoft.com/office/2006/metadata/properties" xmlns:xsi="http://www.w3.org/2001/XMLSchema-instance" xmlns:pc="http://schemas.microsoft.com/office/infopath/2007/PartnerControls">
-  <documentManagement>
-    <MigrationWizIdPermissions xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
-    <MigrationWizIdPermissionLevels xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
-    <MigrationWizIdDocumentLibraryPermissions xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
-    <MigrationWizIdSecurityGroups xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
-    <MigrationWizId xmlns="e3c1d424-5c4e-4dde-982c-2e7112ac5201" xsi:nil="true"/>
-  </documentManagement>
-</p:properties>
+<?mso-contentType ?>
+<FormTemplates xmlns="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms">
+  <Display>DocumentLibraryForm</Display>
+  <Edit>DocumentLibraryForm</Edit>
+  <New>DocumentLibraryForm</New>
+</FormTemplates>
 </file>
 
 <file path=customXml/itemProps1.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8A51473-3926-474A-B0A4-2C7C84CC84DA}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7537FF06-7D0F-4794-9610-42075F4E6CD2}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
+    <ds:schemaRef ds:uri="80e2c8ce-ca24-4d64-a7ff-1f3dbec7935c"/>
+    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
+    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
+    <ds:schemaRef ds:uri="e3c1d424-5c4e-4dde-982c-2e7112ac5201"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
+    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
@@ -20331,18 +20350,9 @@
 </file>
 
 <file path=customXml/itemProps3.xml><?xml version="1.0" encoding="utf-8"?>
-<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{7537FF06-7D0F-4794-9610-42075F4E6CD2}">
+<ds:datastoreItem xmlns:ds="http://schemas.openxmlformats.org/officeDocument/2006/customXml" ds:itemID="{A8A51473-3926-474A-B0A4-2C7C84CC84DA}">
   <ds:schemaRefs>
-    <ds:schemaRef ds:uri="http://purl.org/dc/dcmitype/"/>
-    <ds:schemaRef ds:uri="80e2c8ce-ca24-4d64-a7ff-1f3dbec7935c"/>
-    <ds:schemaRef ds:uri="http://www.w3.org/XML/1998/namespace"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/documentManagement/types"/>
-    <ds:schemaRef ds:uri="http://schemas.openxmlformats.org/package/2006/metadata/core-properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/terms/"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/infopath/2007/PartnerControls"/>
-    <ds:schemaRef ds:uri="e3c1d424-5c4e-4dde-982c-2e7112ac5201"/>
-    <ds:schemaRef ds:uri="http://schemas.microsoft.com/office/2006/metadata/properties"/>
-    <ds:schemaRef ds:uri="http://purl.org/dc/elements/1.1/"/>
+    <ds:schemaRef ds:uri="http://schemas.microsoft.com/sharepoint/v3/contenttype/forms"/>
   </ds:schemaRefs>
 </ds:datastoreItem>
 </file>
</xml_diff>

<commit_message>
add main_start from products for stringers
</commit_message>
<xml_diff>
--- a/scripts/data/Job Ship Dates.xlsx
+++ b/scripts/data/Job Ship Dates.xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PMiller1\git\prodctrlcore\scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{BF07708C-0590-4FE0-B3DC-D3ADBD99EFB6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{CA8B29F5-5489-4DDE-9BBC-167698C1B5A6}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="1305" yWindow="2130" windowWidth="21600" windowHeight="11385" activeTab="3" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="28680" yWindow="-30" windowWidth="29040" windowHeight="16440" activeTab="2" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Dates" sheetId="1" r:id="rId1"/>
@@ -781,7 +781,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43990.341805671298" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.394117708332" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="2">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
@@ -1454,7 +1454,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43990.341809490739" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.394121064812" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
@@ -2142,7 +2142,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43990.341814467596" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.394125115738" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
@@ -2831,7 +2831,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43990.341819328707" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.394129398148" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
@@ -5659,7 +5659,7 @@
     </i>
     <i>
       <x v="166"/>
-      <x v="3"/>
+      <x v="5"/>
     </i>
     <i>
       <x v="167"/>
@@ -9886,8 +9886,8 @@
   <sheetPr codeName="Sheet1"/>
   <dimension ref="A1:C200"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection sqref="A1:C1"/>
+    <sheetView topLeftCell="A166" workbookViewId="0">
+      <selection activeCell="B182" sqref="B182"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -13476,7 +13476,7 @@
         <v>167</v>
       </c>
       <c r="B168" t="s">
-        <v>212</v>
+        <v>221</v>
       </c>
     </row>
     <row r="169" spans="1:2" x14ac:dyDescent="0.25">
@@ -13750,8 +13750,8 @@
   <sheetPr codeName="Sheet3"/>
   <dimension ref="A1:C205"/>
   <sheetViews>
-    <sheetView workbookViewId="0">
-      <selection activeCell="D21" sqref="D21"/>
+    <sheetView tabSelected="1" topLeftCell="A163" workbookViewId="0">
+      <selection activeCell="A184" sqref="A184:XFD184"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
@@ -16039,8 +16039,8 @@
   <sheetPr codeName="Sheet4"/>
   <dimension ref="A1:C361"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A5" sqref="A5"/>
+    <sheetView topLeftCell="A295" workbookViewId="0">
+      <selection activeCell="A325" sqref="A325:XFD325"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>

</xml_diff>

<commit_message>
redid monday using moncli, moves sched parser
</commit_message>
<xml_diff>
--- a/scripts/data/Job Ship Dates.xlsx
+++ b/scripts/data/Job Ship Dates.xlsx
@@ -8,7 +8,7 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\PMiller1\git\prodctrlcore\scripts\data\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{EE806DE6-BCF5-4C9E-BDB3-91C2C3EB833C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{2AA0A7A3-9674-495E-9F21-235EAB8A857C}" xr6:coauthVersionLast="44" xr6:coauthVersionMax="44" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="29580" yWindow="780" windowWidth="21600" windowHeight="11835" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -781,7 +781,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition1.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.459327777775" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.649900925928" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF00000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="2">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
@@ -1454,7 +1454,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition2.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.45933287037" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.649905787039" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF01000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
@@ -2142,7 +2142,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition3.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.459338541667" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.64991122685" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF02000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="4">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">
@@ -2831,7 +2831,7 @@
 </file>
 
 <file path=xl/pivotCache/pivotCacheDefinition4.xml><?xml version="1.0" encoding="utf-8"?>
-<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.459344212963" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
+<pivotCacheDefinition xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="xr" saveData="0" refreshOnLoad="1" refreshedBy="Miller, Pat" refreshedDate="43994.649916435184" backgroundQuery="1" createdVersion="6" refreshedVersion="6" minRefreshableVersion="3" recordCount="0" supportSubquery="1" supportAdvancedDrill="1" xr:uid="{00000000-000A-0000-FFFF-FFFF03000000}">
   <cacheSource type="external" connectionId="1"/>
   <cacheFields count="3">
     <cacheField name="[Job Shipments].[Job Structure Shipment].[Job Structure Shipment]" caption="Job Structure Shipment" numFmtId="0" hierarchy="45" level="1">

</xml_diff>